<commit_message>
Updated Task list to include tasks for the next meeting
Tasks can be found on the sheet marked Tasks 01-28 to 02-04
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TaskList" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="138">
   <si>
     <t>Feature</t>
   </si>
@@ -248,12 +249,6 @@
     <t>Enemy Dies</t>
   </si>
   <si>
-    <t>Ground Enemy</t>
-  </si>
-  <si>
-    <t>Flying Enemy</t>
-  </si>
-  <si>
     <t>Create Enemy Sprites</t>
   </si>
   <si>
@@ -323,23 +318,134 @@
     <t>A base enemy class with generic movement and attack</t>
   </si>
   <si>
-    <t>The ground enemy type</t>
-  </si>
-  <si>
-    <t>The Flying enemy type</t>
-  </si>
-  <si>
     <t>Create HUD, button, and any background graphics</t>
   </si>
   <si>
     <t>Graphics for buttons, the HUD, and any menu or combat backgrounds</t>
+  </si>
+  <si>
+    <t>Learn about JsonFx</t>
+  </si>
+  <si>
+    <t>Time Estimated to Complete</t>
+  </si>
+  <si>
+    <t>Time Spent</t>
+  </si>
+  <si>
+    <t>Over/Under</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Base Boss</t>
+  </si>
+  <si>
+    <t>A Base Boss class</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Create MagicIcon class</t>
+  </si>
+  <si>
+    <t>Create CoinIcon class</t>
+  </si>
+  <si>
+    <t>Create RangedIcon class</t>
+  </si>
+  <si>
+    <t>InventoryItem</t>
+  </si>
+  <si>
+    <t>Controls</t>
+  </si>
+  <si>
+    <t>Create HealthControl</t>
+  </si>
+  <si>
+    <t>Create ManaControl</t>
+  </si>
+  <si>
+    <t>Create WeaponControl</t>
+  </si>
+  <si>
+    <t>Create ShieldControl</t>
+  </si>
+  <si>
+    <t>Fill inventory Class with Fake data</t>
+  </si>
+  <si>
+    <t>Total Hours Assigned</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Will not do to much until the enemy is created</t>
+  </si>
+  <si>
+    <t>Create ActionArea</t>
+  </si>
+  <si>
+    <t>Appears when the WeaponControl is in use</t>
+  </si>
+  <si>
+    <t>Create WeaponControl and attach to WeaponControl Game Object</t>
+  </si>
+  <si>
+    <t>Create ShieldControl and attach to ShieldControl Game Object</t>
+  </si>
+  <si>
+    <t>Filter InventoryItems based on itemType for Inventory Scene</t>
+  </si>
+  <si>
+    <t>Select inventoryItem with touch in Inventory Scene</t>
+  </si>
+  <si>
+    <t>Create ComparedItem Game Object</t>
+  </si>
+  <si>
+    <t>Create SelectedItem Game Object</t>
+  </si>
+  <si>
+    <t>Game Object will display the correct equipped item's information</t>
+  </si>
+  <si>
+    <t>Game Object will display the select item's information</t>
+  </si>
+  <si>
+    <t>Reduce rows in Inventory scene and make slots bigger</t>
+  </si>
+  <si>
+    <t>Rearange Inventory Scene UI</t>
+  </si>
+  <si>
+    <t>To show number of health potions and mana potions the player has</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,13 +491,38 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -407,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -475,6 +606,12 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,6 +619,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -756,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +950,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="22">
         <v>1</v>
@@ -848,10 +990,18 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="23">
+        <v>3</v>
+      </c>
+      <c r="D6" s="23">
+        <v>1</v>
+      </c>
+      <c r="E6" s="23">
+        <v>2</v>
+      </c>
       <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -872,7 +1022,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="17">
         <v>1</v>
@@ -881,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -925,7 +1075,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" s="16">
         <v>1</v>
@@ -937,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -950,10 +1100,10 @@
     </row>
     <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14" s="16">
         <v>2</v>
@@ -965,13 +1115,13 @@
         <v>5</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" s="16">
         <v>2</v>
@@ -983,13 +1133,13 @@
         <v>5</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" s="16">
         <v>2</v>
@@ -1001,13 +1151,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" s="16">
         <v>2</v>
@@ -1019,7 +1169,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1053,7 +1203,7 @@
     <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C20" s="16">
         <v>2</v>
@@ -1065,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,7 +1245,7 @@
         <v>5</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1113,7 +1263,7 @@
         <v>10</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1131,7 +1281,7 @@
         <v>10</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1159,7 +1309,7 @@
         <v>8</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1177,13 +1327,13 @@
         <v>4</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29" s="16">
         <v>2</v>
@@ -1195,7 +1345,7 @@
         <v>5</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1223,7 +1373,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1241,7 +1391,7 @@
         <v>5</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1259,7 +1409,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1295,201 +1445,137 @@
         <v>7</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="16">
-        <v>2</v>
-      </c>
-      <c r="D36" s="16">
-        <v>2</v>
-      </c>
-      <c r="E36" s="16">
-        <v>3</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="16">
-        <v>2</v>
-      </c>
-      <c r="D37" s="16">
-        <v>2</v>
-      </c>
-      <c r="E37" s="16">
-        <v>3</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="10"/>
+      <c r="B36" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="17">
+        <v>2</v>
+      </c>
+      <c r="D36" s="17">
+        <v>2</v>
+      </c>
+      <c r="E36" s="17">
+        <v>7</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+    </row>
+    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>111</v>
+      </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="16">
-        <v>3</v>
-      </c>
-      <c r="D40" s="16">
-        <v>1</v>
-      </c>
-      <c r="E40" s="16">
-        <v>1</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="16">
-        <v>1</v>
-      </c>
-      <c r="D41" s="16">
-        <v>2</v>
-      </c>
-      <c r="E41" s="16">
-        <v>3</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="16">
-        <v>1</v>
-      </c>
-      <c r="D42" s="16">
-        <v>1</v>
-      </c>
-      <c r="E42" s="16">
-        <v>6</v>
-      </c>
-      <c r="F42" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="16">
-        <v>1</v>
-      </c>
-      <c r="D43" s="16">
-        <v>3</v>
-      </c>
-      <c r="E43" s="16">
-        <v>6</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="16">
-        <v>2</v>
-      </c>
-      <c r="D44" s="16">
-        <v>2</v>
-      </c>
-      <c r="E44" s="16">
-        <v>4</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="16">
-        <v>1</v>
-      </c>
-      <c r="D45" s="16">
-        <v>3</v>
-      </c>
-      <c r="E45" s="16"/>
-      <c r="F45" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="10"/>
+    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+    </row>
+    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+    </row>
+    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+    </row>
+    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+    </row>
+    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+    </row>
+    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+    </row>
+    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="17">
-        <v>2</v>
-      </c>
-      <c r="D47" s="17">
-        <v>2</v>
-      </c>
-      <c r="E47" s="17">
-        <v>3</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>58</v>
-      </c>
+    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
     </row>
     <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
+      <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
@@ -1497,195 +1583,571 @@
       <c r="F48" s="17"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>2</v>
-      </c>
-      <c r="E49">
-        <v>4</v>
-      </c>
-      <c r="F49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="14">
-        <v>1</v>
-      </c>
-      <c r="D50" s="14">
-        <v>2</v>
-      </c>
-      <c r="E50" s="14">
-        <v>1</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="24"/>
+      <c r="A49" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="16">
+        <v>3</v>
+      </c>
+      <c r="D50" s="16">
+        <v>1</v>
+      </c>
+      <c r="E50" s="16">
+        <v>1</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="16">
+        <v>1</v>
+      </c>
+      <c r="D51" s="16">
+        <v>2</v>
+      </c>
+      <c r="E51" s="16">
+        <v>3</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="16">
+        <v>1</v>
+      </c>
+      <c r="D52" s="16">
+        <v>1</v>
+      </c>
+      <c r="E52" s="16">
+        <v>6</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A53" s="4"/>
       <c r="B53" s="9" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C53" s="16">
+        <v>1</v>
+      </c>
+      <c r="D53" s="16">
         <v>3</v>
       </c>
-      <c r="D53" s="16">
-        <v>1</v>
-      </c>
       <c r="E53" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C54" s="16">
+        <v>2</v>
+      </c>
+      <c r="D54" s="16">
+        <v>2</v>
+      </c>
+      <c r="E54" s="16">
         <v>4</v>
       </c>
-      <c r="D54" s="16">
-        <v>1</v>
-      </c>
-      <c r="E54" s="16">
-        <v>1</v>
-      </c>
       <c r="F54" s="15" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="9" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C55" s="16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D55" s="16">
-        <v>1</v>
-      </c>
-      <c r="E55" s="16">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E55" s="16"/>
       <c r="F55" s="15" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="10"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="17">
+        <v>2</v>
+      </c>
+      <c r="D57" s="17">
+        <v>2</v>
+      </c>
+      <c r="E57" s="17">
+        <v>3</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="15"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+      <c r="F59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="15"/>
+      <c r="B60" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="14">
+        <v>1</v>
+      </c>
+      <c r="D60" s="14">
+        <v>2</v>
+      </c>
+      <c r="E60" s="14">
+        <v>1</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="15"/>
+      <c r="B61" s="24"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="16">
+        <v>3</v>
+      </c>
+      <c r="D63" s="16">
+        <v>1</v>
+      </c>
+      <c r="E63" s="16">
+        <v>5</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="16">
+        <v>4</v>
+      </c>
+      <c r="D64" s="16">
+        <v>1</v>
+      </c>
+      <c r="E64" s="16">
+        <v>1</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="16">
+        <v>4</v>
+      </c>
+      <c r="D65" s="16">
+        <v>1</v>
+      </c>
+      <c r="E65" s="16">
+        <v>1</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="16">
+      <c r="C66" s="16">
         <v>3</v>
       </c>
-      <c r="D56" s="16">
+      <c r="D66" s="16">
         <v>3</v>
       </c>
-      <c r="E56" s="16">
+      <c r="E66" s="16">
         <v>4</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F66" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="15" t="s">
+    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="17"/>
+      <c r="B67" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="16">
+      <c r="C67" s="16">
         <v>3</v>
       </c>
-      <c r="D57" s="16">
+      <c r="D67" s="16">
         <v>3</v>
       </c>
-      <c r="E57" s="16">
+      <c r="E67" s="16">
         <v>4</v>
       </c>
-      <c r="F57" s="15" t="s">
+      <c r="F67" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="15" t="s">
+    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="17"/>
+      <c r="B68" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C58" s="16">
+      <c r="C68" s="16">
         <v>3</v>
       </c>
-      <c r="D58" s="16">
+      <c r="D68" s="16">
         <v>3</v>
       </c>
-      <c r="E58" s="16">
+      <c r="E68" s="16">
         <v>4</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F68" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="15" t="s">
+    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="17"/>
+      <c r="B69" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="16">
+      <c r="C69" s="16">
         <v>4</v>
       </c>
-      <c r="D59" s="16">
-        <v>2</v>
-      </c>
-      <c r="E59" s="16">
-        <v>2</v>
-      </c>
-      <c r="F59" s="15" t="s">
+      <c r="D69" s="16">
+        <v>2</v>
+      </c>
+      <c r="E69" s="16">
+        <v>2</v>
+      </c>
+      <c r="F69" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="14"/>
-      <c r="D61" s="20" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C71" s="14"/>
+      <c r="D71" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E61" s="20">
-        <f>SUM(E3:E59)</f>
-        <v>183</v>
-      </c>
-      <c r="F61" s="14"/>
+      <c r="E71" s="20">
+        <f>SUM(E3:E69)</f>
+        <v>186</v>
+      </c>
+      <c r="F71" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" t="s">
+        <v>134</v>
+      </c>
+      <c r="M9" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" t="s">
+        <v>137</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16">
+        <f>SUM(B2:B14)</f>
+        <v>14.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rearranged Inventory scene and updated Level Scene
Fills Inventory class with fake data

Removed some rows from inventory scene, added counts for potions and
made selectitem and compareditem game objects bigger

Added WeaponControl, ActionAera, and ShieldControl to level scene
Added Sky, Ground, and Background game objects to level scene

Removed Common script

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="139">
   <si>
     <t>Feature</t>
   </si>
@@ -426,19 +426,22 @@
     <t>Create SelectedItem Game Object</t>
   </si>
   <si>
-    <t>Game Object will display the correct equipped item's information</t>
-  </si>
-  <si>
     <t>Game Object will display the select item's information</t>
   </si>
   <si>
     <t>Reduce rows in Inventory scene and make slots bigger</t>
   </si>
   <si>
-    <t>Rearange Inventory Scene UI</t>
-  </si>
-  <si>
     <t>To show number of health potions and mana potions the player has</t>
+  </si>
+  <si>
+    <t>Rearrange Inventory Scene UI</t>
+  </si>
+  <si>
+    <t>Game Object will display the correct equipped item's information to compare with the selected item</t>
+  </si>
+  <si>
+    <t>Create Sky,Ground, and Background Game Objects</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +1941,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,7 +1951,7 @@
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1983,11 +1986,14 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
       <c r="E2" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1997,11 +2003,14 @@
       <c r="B3" s="14">
         <v>1</v>
       </c>
+      <c r="C3" s="14">
+        <v>0.5</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>126</v>
@@ -2014,11 +2023,14 @@
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2028,11 +2040,14 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G5" t="s">
         <v>124</v>
@@ -2080,7 +2095,7 @@
         <v>121</v>
       </c>
       <c r="G8" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2097,7 +2112,7 @@
         <v>121</v>
       </c>
       <c r="G9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M9" s="26" t="s">
         <v>121</v>
@@ -2105,16 +2120,19 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10">
         <v>0.5</v>
       </c>
+      <c r="C10">
+        <v>0.25</v>
+      </c>
       <c r="E10" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>121</v>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="M10" s="27" t="s">
         <v>122</v>
@@ -2127,16 +2145,36 @@
       <c r="B11">
         <v>0.5</v>
       </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
       <c r="E11" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>121</v>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.25</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2146,7 +2184,11 @@
       </c>
       <c r="B16">
         <f>SUM(B2:B14)</f>
-        <v>14.5</v>
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C2:C15)</f>
+        <v>4.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Inventory Scene, Expanded Numerous Base Classes
Added ComparedItem and SelectedItem Game Objects to inventory scene that
display selected and compared items
Added working inventoryslots that display the Player's unequipped items

Added Constructor and ToString method to InventoryItem and All it's
derived classes

updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="140">
   <si>
     <t>Feature</t>
   </si>
@@ -442,6 +442,9 @@
   </si>
   <si>
     <t>Create Sky,Ground, and Background Game Objects</t>
+  </si>
+  <si>
+    <t>Convert unequippedItems to a List</t>
   </si>
 </sst>
 </file>
@@ -1941,7 +1944,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,11 +2063,14 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2074,11 +2080,14 @@
       <c r="B7">
         <v>1.5</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2088,6 +2097,9 @@
       <c r="B8">
         <v>2</v>
       </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
@@ -2105,6 +2117,9 @@
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
@@ -2178,17 +2193,31 @@
         <v>123</v>
       </c>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>120</v>
       </c>
       <c r="B16">
         <f>SUM(B2:B14)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <f>SUM(C2:C15)</f>
-        <v>4.75</v>
+        <v>10.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted unequippedItems into a List, Improved Item Equipping
Converted unequippedItems into a List

Improved Item Equipping

Expanded ResetBoard method in InventoryScript

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -1944,7 +1944,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,8 +2103,8 @@
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
+      <c r="F8" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -2118,13 +2118,13 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>121</v>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G9" t="s">
         <v>133</v>
@@ -2200,11 +2200,14 @@
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13">
+        <v>0.25</v>
+      </c>
       <c r="E13" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>121</v>
+      <c r="F13" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2217,7 +2220,7 @@
       </c>
       <c r="C16">
         <f>SUM(C2:C15)</f>
-        <v>10.75</v>
+        <v>11.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Icon Class, and Updated IconSpawner
Base Icon Class created
IconSpawner spawns in base icon class using IconPrefab
Updated TaskList
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="142">
   <si>
     <t>Feature</t>
   </si>
@@ -438,13 +438,19 @@
     <t>Rearrange Inventory Scene UI</t>
   </si>
   <si>
-    <t>Game Object will display the correct equipped item's information to compare with the selected item</t>
-  </si>
-  <si>
     <t>Create Sky,Ground, and Background Game Objects</t>
   </si>
   <si>
     <t>Convert unequippedItems to a List</t>
+  </si>
+  <si>
+    <t>Create Icon Base Class</t>
+  </si>
+  <si>
+    <t>Still need to alter to show compared magic when looking at magic section</t>
+  </si>
+  <si>
+    <t>Icon Spawner can spawn these in</t>
   </si>
 </sst>
 </file>
@@ -1944,7 +1950,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,7 +2113,7 @@
         <v>122</v>
       </c>
       <c r="G8" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2178,7 +2184,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12">
         <v>0.5</v>
@@ -2195,7 +2201,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2208,6 +2214,26 @@
       </c>
       <c r="F13" s="28" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2216,11 +2242,11 @@
       </c>
       <c r="B16">
         <f>SUM(B2:B14)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <f>SUM(C2:C15)</f>
-        <v>11.25</v>
+        <v>13.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Task list, Icons, and Controls
Only one icon can be selected at a time now (had to update
icon,shieldcontrol, and weaponcontrol)

Updated task list to include next weeks tasks
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId2"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="154">
   <si>
     <t>Feature</t>
   </si>
@@ -451,6 +452,42 @@
   </si>
   <si>
     <t>Icon Spawner can spawn these in</t>
+  </si>
+  <si>
+    <t>Create MagicIcon</t>
+  </si>
+  <si>
+    <t>Create CoinIcon</t>
+  </si>
+  <si>
+    <t>Create RangedIcon</t>
+  </si>
+  <si>
+    <t>Create Base Enemy Class</t>
+  </si>
+  <si>
+    <t>Create EnemySpawner</t>
+  </si>
+  <si>
+    <t>Base Enemy class will have basic enemy behaviours</t>
+  </si>
+  <si>
+    <t>Will Spawn in Enemy Prefab</t>
+  </si>
+  <si>
+    <t>Create EnemyPrefab</t>
+  </si>
+  <si>
+    <t>Adds a coin when colliding with coinbag</t>
+  </si>
+  <si>
+    <t>Add iconselect boolean to prevent multiple icons being selected</t>
+  </si>
+  <si>
+    <t>Add a RigidBody to the base icon</t>
+  </si>
+  <si>
+    <t>Have IconSpawner Spawn in new icons when old ones are used</t>
   </si>
 </sst>
 </file>
@@ -1947,10 +1984,265 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="14">
+        <f>SUM(B3:B10)</f>
+        <v>15</v>
+      </c>
+      <c r="C13" s="14">
+        <f>SUM(C3:C12)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,6 +2290,9 @@
       <c r="C2">
         <v>0.5</v>
       </c>
+      <c r="D2">
+        <v>-0.5</v>
+      </c>
       <c r="E2" t="s">
         <v>106</v>
       </c>
@@ -2015,6 +2310,9 @@
       <c r="C3" s="14">
         <v>0.5</v>
       </c>
+      <c r="D3" s="14">
+        <v>-0.5</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
@@ -2035,6 +2333,9 @@
       <c r="C4">
         <v>2</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
@@ -2052,6 +2353,9 @@
       <c r="C5">
         <v>1</v>
       </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
@@ -2072,6 +2376,9 @@
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
@@ -2089,6 +2396,9 @@
       <c r="C7">
         <v>1</v>
       </c>
+      <c r="D7">
+        <v>-0.5</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
@@ -2106,6 +2416,9 @@
       <c r="C8">
         <v>2</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
@@ -2126,6 +2439,9 @@
       <c r="C9">
         <v>1.25</v>
       </c>
+      <c r="D9">
+        <v>-0.75</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
@@ -2149,6 +2465,9 @@
       <c r="C10">
         <v>0.25</v>
       </c>
+      <c r="D10">
+        <v>-0.25</v>
+      </c>
       <c r="E10" s="14" t="s">
         <v>106</v>
       </c>
@@ -2169,6 +2488,9 @@
       <c r="C11">
         <v>0.25</v>
       </c>
+      <c r="D11">
+        <v>-0.25</v>
+      </c>
       <c r="E11" s="14" t="s">
         <v>106</v>
       </c>
@@ -2192,6 +2514,9 @@
       <c r="C12">
         <v>0.25</v>
       </c>
+      <c r="D12">
+        <v>-0.25</v>
+      </c>
       <c r="E12" s="14" t="s">
         <v>106</v>
       </c>
@@ -2209,6 +2534,9 @@
       <c r="C13">
         <v>0.25</v>
       </c>
+      <c r="D13">
+        <v>-0.75</v>
+      </c>
       <c r="E13" s="14" t="s">
         <v>106</v>
       </c>
@@ -2225,6 +2553,9 @@
       </c>
       <c r="C14">
         <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Script Cleanup, added rigidbody to icon, Updated Task List
Cleaned up some scripts
Added a rigidbody to the icon for fluid movement after the icon is let
go
updated the task list
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="155">
   <si>
     <t>Feature</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>Have IconSpawner Spawn in new icons when old ones are used</t>
+  </si>
+  <si>
+    <t>Script Cleanup</t>
   </si>
 </sst>
 </file>
@@ -1984,10 +1987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,13 +2032,17 @@
       <c r="B2" s="25">
         <v>0.5</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="25">
+        <v>0</v>
+      </c>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G2" s="25"/>
     </row>
@@ -2044,7 +2051,7 @@
         <v>142</v>
       </c>
       <c r="B3" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -2061,7 +2068,7 @@
         <v>143</v>
       </c>
       <c r="B4" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -2080,7 +2087,7 @@
         <v>144</v>
       </c>
       <c r="B5" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2111,7 +2118,7 @@
         <v>145</v>
       </c>
       <c r="B7" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2176,8 +2183,8 @@
       <c r="E10" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>122</v>
+      <c r="F10" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>140</v>
@@ -2206,31 +2213,48 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="14">
-        <f>SUM(B3:B10)</f>
-        <v>15</v>
-      </c>
-      <c r="C13" s="14">
-        <f>SUM(C3:C12)</f>
-        <v>0.25</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="14">
+        <f>SUM(B3:B10)</f>
+        <v>14</v>
+      </c>
+      <c r="C14" s="14">
+        <f>SUM(C3:C13)</f>
+        <v>0.75</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2241,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added MagicIcon, RangedIcon, and CoinIcon, updated IconSpawner
Magic, Ranged, and Coin Icons now spawn in, currently spawn in at random
(stamina and mana will go down when they are used)
Coin Bag will accept coin icons now
Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -1990,7 +1990,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,13 +2053,17 @@
       <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G3" s="14"/>
     </row>
@@ -2070,13 +2074,17 @@
       <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-0.5</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>150</v>
@@ -2089,13 +2097,17 @@
       <c r="B5" s="14">
         <v>1</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.5</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G5" s="14"/>
     </row>
@@ -2109,8 +2121,8 @@
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
+      <c r="F6" s="27" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2125,8 +2137,8 @@
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
+      <c r="F7" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>147</v>
@@ -2142,8 +2154,8 @@
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
+      <c r="F8" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>121</v>
@@ -2161,8 +2173,8 @@
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>121</v>
+      <c r="F9" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>148</v>
@@ -2249,7 +2261,7 @@
       </c>
       <c r="C14" s="14">
         <f>SUM(C3:C13)</f>
-        <v>0.75</v>
+        <v>3.75</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>

</xml_diff>

<commit_message>
Cleaned up some scripts, Created Base Enemy Class and Enemy Spawner
Cleaned up up some scripts

Created base enemy class and prefab (Known issue with colliders
preventing MeleeWeapon from damaging enemy)

Created Enemy Spawner that controls end of game

Updated MeleeWeapon to take in prefab of weapon as a parameter
Updated LevelScript to instantiate prefab of attached meleeweapon

Added DealDamage method to Magic and Weapons and BlockDamage method to
Shield

Added isDefending variable to Player class for using shield

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -1990,7 +1990,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,8 +2132,12 @@
       <c r="B7" s="14">
         <v>5</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="14">
+        <v>6</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
@@ -2151,11 +2155,17 @@
       <c r="B8" s="14">
         <v>0.5</v>
       </c>
+      <c r="C8" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>122</v>
+      <c r="F8" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>121</v>
@@ -2168,13 +2178,17 @@
       <c r="B9" s="14">
         <v>1</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>122</v>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>148</v>
@@ -2230,10 +2244,10 @@
         <v>154</v>
       </c>
       <c r="B12" s="14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C12" s="14">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D12" s="14">
         <v>0</v>
@@ -2261,7 +2275,7 @@
       </c>
       <c r="C14" s="14">
         <f>SUM(C3:C13)</f>
-        <v>3.75</v>
+        <v>12.25</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>

</xml_diff>

<commit_message>
Added some basic icon respawning and added new tasks to the Task List
New Tasks in the task list
Some basic icon respawning (more elaborate setup to come)
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId2"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId3"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId2"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId3"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="163">
   <si>
     <t>Feature</t>
   </si>
@@ -469,9 +470,6 @@
     <t>Create EnemySpawner</t>
   </si>
   <si>
-    <t>Base Enemy class will have basic enemy behaviours</t>
-  </si>
-  <si>
     <t>Will Spawn in Enemy Prefab</t>
   </si>
   <si>
@@ -491,6 +489,33 @@
   </si>
   <si>
     <t>Script Cleanup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expand MagicIcon class </t>
+  </si>
+  <si>
+    <t>Create FlyingEnemy Class</t>
+  </si>
+  <si>
+    <t>Create StandingEnemy Class</t>
+  </si>
+  <si>
+    <t>Create Base Boss Class</t>
+  </si>
+  <si>
+    <t>Issue occurring with collisions</t>
+  </si>
+  <si>
+    <t>Fix Icons and enemies colliding with each other</t>
+  </si>
+  <si>
+    <t>Fix Base Enemy Collisions with weapon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will be like a wolf </t>
+  </si>
+  <si>
+    <t>And make variables public</t>
   </si>
 </sst>
 </file>
@@ -1987,10 +2012,233 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="14">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="14">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>19.5</v>
+      </c>
+      <c r="C11" s="14">
+        <f>SUM(C2:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2275,7 @@
     </row>
     <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="25">
         <v>0.5</v>
@@ -2087,7 +2335,7 @@
         <v>123</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2113,10 +2361,13 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6" s="14">
         <v>2.5</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.5</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
@@ -2145,12 +2396,12 @@
         <v>122</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" s="14">
         <v>0.5</v>
@@ -2191,7 +2442,7 @@
         <v>123</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H9" s="27" t="s">
         <v>122</v>
@@ -2221,7 +2472,7 @@
     </row>
     <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="14">
         <v>0.25</v>
@@ -2241,7 +2492,7 @@
     </row>
     <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="14">
         <v>1</v>
@@ -2275,7 +2526,7 @@
       </c>
       <c r="C14" s="14">
         <f>SUM(C3:C13)</f>
-        <v>12.25</v>
+        <v>12.75</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -2287,7 +2538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added a Finite State Machine class, updated Enemy class
Updated Enemy prefab to have some public variables
Added a Finite State Machine to the Enemy class
Reduced code coupling in Enemy class

Updated Player and PlayerStats classes

Introduced collision detection to Icon class (allows icons to handle
collisions with enemy or player)

Changed all OnCollisionEnter2D methods to OnTriggerEnter2D

Renamed some files

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityGames\RPGHeroPrototype\TechnicalDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\UnityGames\RPGHeroPrototype\TechnicalDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="167">
   <si>
     <t>Feature</t>
   </si>
@@ -518,16 +518,16 @@
     <t>And make variables public</t>
   </si>
   <si>
-    <t>Have things that are being effected deal with it themselves(Such as player handle being attacked</t>
-  </si>
-  <si>
-    <t>Finite state machine for enemy</t>
-  </si>
-  <si>
-    <t>Reduce coupling(enemy shouldn't know about icon logic) introduce a OnHit Method</t>
-  </si>
-  <si>
     <t>Change name of enemy methods to OnXXX</t>
+  </si>
+  <si>
+    <t>Update MeleeWeapon to take in a prefab and itemImage</t>
+  </si>
+  <si>
+    <t>Reduce coupling/Clean up code</t>
+  </si>
+  <si>
+    <t>Research and implement Finite state machine for enemy</t>
   </si>
 </sst>
 </file>
@@ -993,15 +993,15 @@
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" customWidth="1"/>
-    <col min="6" max="6" width="255.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="255.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="13"/>
       <c r="C4" s="23"/>
@@ -1059,7 +1059,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="13" t="s">
         <v>99</v>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1103,7 +1103,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1131,7 +1131,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="10"/>
       <c r="C11" s="17"/>
@@ -1159,7 +1159,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
@@ -1187,7 +1187,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>81</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
         <v>83</v>
@@ -1225,7 +1225,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
         <v>84</v>
@@ -1243,7 +1243,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15" t="s">
         <v>85</v>
@@ -1261,7 +1261,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="10"/>
       <c r="C18" s="17"/>
@@ -1269,7 +1269,7 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="9" t="s">
         <v>97</v>
@@ -1307,7 +1307,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="9" t="s">
         <v>63</v>
@@ -1355,7 +1355,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="9" t="s">
         <v>64</v>
@@ -1373,7 +1373,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1381,7 +1381,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>71</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="9" t="s">
         <v>72</v>
@@ -1419,7 +1419,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="9" t="s">
         <v>90</v>
@@ -1437,7 +1437,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="10"/>
       <c r="C30" s="17"/>
@@ -1445,7 +1445,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>65</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="9" t="s">
         <v>67</v>
@@ -1483,7 +1483,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="9" t="s">
         <v>68</v>
@@ -1501,7 +1501,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="9" t="s">
         <v>70</v>
@@ -1519,7 +1519,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="9" t="s">
         <v>69</v>
@@ -1537,7 +1537,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="10" t="s">
         <v>107</v>
@@ -1555,7 +1555,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -1563,7 +1563,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>109</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>110</v>
@@ -1585,7 +1585,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>112</v>
@@ -1595,7 +1595,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -1603,7 +1603,7 @@
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>113</v>
       </c>
@@ -1613,7 +1613,7 @@
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -1621,7 +1621,7 @@
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
     </row>
-    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>114</v>
       </c>
@@ -1633,7 +1633,7 @@
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
     </row>
-    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>116</v>
@@ -1643,7 +1643,7 @@
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>117</v>
@@ -1653,7 +1653,7 @@
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
     </row>
-    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>118</v>
@@ -1663,7 +1663,7 @@
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -1671,7 +1671,7 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>11</v>
       </c>
@@ -1681,7 +1681,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>13</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="9" t="s">
         <v>41</v>
@@ -1719,7 +1719,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="9" t="s">
         <v>44</v>
@@ -1737,7 +1737,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="9" t="s">
         <v>45</v>
@@ -1755,7 +1755,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="9" t="s">
         <v>46</v>
@@ -1773,7 +1773,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="9" t="s">
         <v>47</v>
@@ -1789,7 +1789,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="10"/>
       <c r="C56" s="17"/>
@@ -1797,7 +1797,7 @@
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>14</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -1825,7 +1825,7 @@
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>15</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="14" t="s">
         <v>54</v>
@@ -1863,11 +1863,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
       <c r="B61" s="24"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>16</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>17</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="9" t="s">
         <v>19</v>
@@ -1915,7 +1915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="9" t="s">
         <v>20</v>
@@ -1933,7 +1933,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="9" t="s">
         <v>33</v>
@@ -1951,7 +1951,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="15" t="s">
         <v>31</v>
@@ -1969,7 +1969,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17"/>
       <c r="B68" s="15" t="s">
         <v>32</v>
@@ -1987,7 +1987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17"/>
       <c r="B69" s="15" t="s">
         <v>34</v>
@@ -2005,7 +2005,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C71" s="14"/>
       <c r="D71" s="20" t="s">
         <v>21</v>
@@ -2027,19 +2027,19 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>154</v>
       </c>
@@ -2081,45 +2081,53 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>152</v>
       </c>
       <c r="B3" s="14">
         <v>1.5</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="14">
+        <v>-1</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="27" t="s">
-        <v>122</v>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>160</v>
       </c>
       <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-0.5</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>122</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>162</v>
       </c>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>156</v>
       </c>
@@ -2136,7 +2144,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>155</v>
       </c>
@@ -2150,7 +2158,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>157</v>
       </c>
@@ -2164,7 +2172,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>131</v>
       </c>
@@ -2183,45 +2191,98 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>159</v>
       </c>
       <c r="B9" s="14">
         <v>3</v>
       </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>-2</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="14">
+        <v>4</v>
+      </c>
+      <c r="C10" s="14">
+        <v>4</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F10" s="27"/>
-    </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="F11" s="27"/>
-    </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="14">
+        <v>2</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2.25</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="F12" s="27"/>
-    </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+        <v>164</v>
+      </c>
+      <c r="B13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -2231,17 +2292,17 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>120</v>
       </c>
       <c r="B15" s="14">
-        <f>SUM(B2:B9)</f>
-        <v>19.5</v>
+        <f>SUM(B2:B13)</f>
+        <v>26.25</v>
       </c>
       <c r="C15" s="14">
         <f>SUM(C2:C14)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -2249,17 +2310,17 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L21" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L22" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L23" s="28" t="s">
         <v>123</v>
       </c>
@@ -2277,16 +2338,16 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.265625" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2309,7 +2370,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>151</v>
       </c>
@@ -2330,7 +2391,7 @@
       </c>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>142</v>
       </c>
@@ -2351,7 +2412,7 @@
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>143</v>
       </c>
@@ -2374,7 +2435,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>144</v>
       </c>
@@ -2395,7 +2456,7 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>152</v>
       </c>
@@ -2412,7 +2473,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>145</v>
       </c>
@@ -2435,7 +2496,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>148</v>
       </c>
@@ -2458,7 +2519,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>146</v>
       </c>
@@ -2484,7 +2545,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>131</v>
       </c>
@@ -2506,7 +2567,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>150</v>
       </c>
@@ -2526,7 +2587,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>153</v>
       </c>
@@ -2543,7 +2604,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -2552,7 +2613,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>120</v>
       </c>
@@ -2582,19 +2643,19 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.73046875" customWidth="1"/>
-    <col min="3" max="3" width="14.1328125" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.73046875" customWidth="1"/>
-    <col min="13" max="13" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2617,7 +2678,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -2637,7 +2698,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>125</v>
       </c>
@@ -2660,7 +2721,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -2680,7 +2741,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -2703,7 +2764,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -2723,7 +2784,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -2743,7 +2804,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -2766,7 +2827,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -2792,7 +2853,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -2815,7 +2876,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -2841,7 +2902,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -2861,7 +2922,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -2881,7 +2942,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -2904,7 +2965,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Worked on managing Level State with Finite State Machine
Worked on Level State by having EnemySpawner and IconSpawner call
methods when the level is in a certain state

Icons now disappear when they are no longer visible (also improved icon
spawning)

Updated Task List with new tasks
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId2"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId3"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId4"/>
+    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId2"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId3"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId4"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="174">
   <si>
     <t>Feature</t>
   </si>
@@ -528,6 +529,27 @@
   </si>
   <si>
     <t>Research and implement Finite state machine for enemy</t>
+  </si>
+  <si>
+    <t>Destroy Icons after leaving the camera</t>
+  </si>
+  <si>
+    <t>Have Multiple methods called on certain situations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue with changing state </t>
+  </si>
+  <si>
+    <t>Implement Fire and Ice Spells</t>
+  </si>
+  <si>
+    <t>Like a Eagle</t>
+  </si>
+  <si>
+    <t>Will have a special attack</t>
+  </si>
+  <si>
+    <t>Fix any troubles discovered during meeting</t>
   </si>
 </sst>
 </file>
@@ -2024,10 +2046,384 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="14">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="14">
+        <v>4</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="14">
+        <f>SUM(B2:B8)</f>
+        <v>17</v>
+      </c>
+      <c r="C10" s="14">
+        <f>SUM(C2:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2258,6 +2654,9 @@
       <c r="C12" s="14">
         <v>0.25</v>
       </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
       <c r="E12" s="14" t="s">
         <v>106</v>
       </c>
@@ -2275,6 +2674,9 @@
       <c r="C13" s="14">
         <v>0.5</v>
       </c>
+      <c r="D13" s="14">
+        <v>0</v>
+      </c>
       <c r="E13" s="14" t="s">
         <v>106</v>
       </c>
@@ -2282,46 +2684,86 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="14">
+        <v>4</v>
+      </c>
+      <c r="C15" s="14">
+        <v>3</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="14">
-        <f>SUM(B2:B13)</f>
-        <v>26.25</v>
-      </c>
-      <c r="C15" s="14">
-        <f>SUM(C2:C14)</f>
-        <v>9</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L21" s="26" t="s">
+      <c r="B17" s="14">
+        <f>SUM(B2:B15)</f>
+        <v>30.5</v>
+      </c>
+      <c r="C17" s="14">
+        <f>SUM(C2:C16)</f>
+        <v>12.25</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L22" s="27" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L23" s="28" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2330,7 +2772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -2635,7 +3077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Moved Level State Code out of LevelScript and into LevelStateManager
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="178">
   <si>
     <t>Feature</t>
   </si>
@@ -534,15 +534,9 @@
     <t>Destroy Icons after leaving the camera</t>
   </si>
   <si>
-    <t>Have Multiple methods called on certain situations</t>
-  </si>
-  <si>
     <t xml:space="preserve">Issue with changing state </t>
   </si>
   <si>
-    <t>Implement Fire and Ice Spells</t>
-  </si>
-  <si>
     <t>Like a Eagle</t>
   </si>
   <si>
@@ -550,6 +544,24 @@
   </si>
   <si>
     <t>Fix any troubles discovered during meeting</t>
+  </si>
+  <si>
+    <t>Incorporate the FiniteStateMachine into the level to store levelstate</t>
+  </si>
+  <si>
+    <t>Move Level State code into a separate class and fix and implementation issues</t>
+  </si>
+  <si>
+    <t>fix any issues with the Finite state machine for the enemy</t>
+  </si>
+  <si>
+    <t>Create FireSpell Class</t>
+  </si>
+  <si>
+    <t>Create FrostSpell Class</t>
+  </si>
+  <si>
+    <t>Alter ComparedItem Class to display equipped Magic</t>
   </si>
 </sst>
 </file>
@@ -2046,15 +2058,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -2093,10 +2105,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="B2" s="14">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -2106,45 +2118,33 @@
       <c r="F2" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>170</v>
-      </c>
+      <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="B3" s="14">
-        <v>2</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+        <v>1.5</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B4" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -2155,7 +2155,7 @@
         <v>121</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -2165,10 +2165,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2179,7 +2179,7 @@
         <v>121</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -2189,10 +2189,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="B6" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2203,7 +2203,7 @@
         <v>121</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -2213,21 +2213,21 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="27" t="s">
-        <v>122</v>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -2237,12 +2237,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B8" s="14">
-        <v>2</v>
-      </c>
-      <c r="C8" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0.25</v>
+      </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14" t="s">
         <v>106</v>
@@ -2251,7 +2253,7 @@
         <v>122</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2260,13 +2262,25 @@
       <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0.5</v>
+      </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -2274,17 +2288,9 @@
       <c r="L9" s="14"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="14">
-        <f>SUM(B2:B8)</f>
-        <v>17</v>
-      </c>
-      <c r="C10" s="14">
-        <f>SUM(C2:C9)</f>
-        <v>0</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -2296,9 +2302,17 @@
       <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>17</v>
+      </c>
+      <c r="C11" s="14">
+        <f>SUM(C2:C10)</f>
+        <v>0.75</v>
+      </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -2377,9 +2391,7 @@
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="26" t="s">
-        <v>121</v>
-      </c>
+      <c r="L16" s="14"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
@@ -2393,8 +2405,8 @@
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="27" t="s">
-        <v>122</v>
+      <c r="L17" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2409,7 +2421,23 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="28" t="s">
+      <c r="L18" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2423,7 +2451,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2706,7 +2734,7 @@
     </row>
     <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B15" s="14">
         <v>4</v>
@@ -2721,7 +2749,7 @@
         <v>122</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added FireBlast and FrostBlast Magic
Added FireBlast and FrostBlast which derive Magic

Updated Magic class and MagicIcon

Updated Inventory class to use FireBlast and FrostBlast

Updated IconSpawner

Updated TaskList
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -2061,7 +2061,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,13 +2110,15 @@
       <c r="B2" s="14">
         <v>1.5</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="14">
+        <v>1.25</v>
+      </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
+      <c r="F2" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -2132,11 +2134,14 @@
       <c r="B3" s="14">
         <v>1.5</v>
       </c>
+      <c r="C3" s="14">
+        <v>0.5</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
+      <c r="F3" s="27" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2311,7 +2316,7 @@
       </c>
       <c r="C11" s="14">
         <f>SUM(C2:C10)</f>
-        <v>0.75</v>
+        <v>2.5</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>

</xml_diff>

<commit_message>
Updated Enemy, Magic, and Weapon. Improved IconSpawner. added Fire and Frost Blast
Reduced coupling in Enemy class
Added TakeDamage, TakeDamageOverTime, and SlowDown to Enemy class

Updated Weapon class

Updated Magic class
Added FireBlastMagic and FrostBlastMagic

Improved IconSpawner

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId2"/>
-    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId3"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId4"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId5"/>
+    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId2"/>
+    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId3"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId4"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId5"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="181">
   <si>
     <t>Feature</t>
   </si>
@@ -562,6 +563,15 @@
   </si>
   <si>
     <t>Alter ComparedItem Class to display equipped Magic</t>
+  </si>
+  <si>
+    <t>Ran into issue with slowing enemy</t>
+  </si>
+  <si>
+    <t>Add Health Bar to enemy class</t>
+  </si>
+  <si>
+    <t>Fix issue of IconSpawner always spawning FrostBlast Icons</t>
   </si>
 </sst>
 </file>
@@ -2058,10 +2068,325 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="14">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="14">
+        <v>4</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="14">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="14">
+        <f>SUM(B2:B6)</f>
+        <v>13</v>
+      </c>
+      <c r="C8" s="14">
+        <f>SUM(C2:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,14 +2436,14 @@
         <v>1.5</v>
       </c>
       <c r="C2" s="14">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>122</v>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -2135,13 +2460,16 @@
         <v>1.5</v>
       </c>
       <c r="C3" s="14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="27" t="s">
-        <v>122</v>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2156,8 +2484,8 @@
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
+      <c r="F4" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>161</v>
@@ -2248,7 +2576,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="14">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14" t="s">
@@ -2292,32 +2620,27 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="14">
-        <f>SUM(B2:B9)</f>
-        <v>17</v>
-      </c>
-      <c r="C11" s="14">
-        <f>SUM(C2:C10)</f>
-        <v>2.5</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -2329,9 +2652,17 @@
       <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="14">
+        <f>SUM(B2:B10)</f>
+        <v>17.5</v>
+      </c>
+      <c r="C12" s="14">
+        <f>SUM(C2:C11)</f>
+        <v>6</v>
+      </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -2410,9 +2741,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="26" t="s">
-        <v>121</v>
-      </c>
+      <c r="L17" s="14"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
@@ -2426,8 +2755,8 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="27" t="s">
-        <v>122</v>
+      <c r="L18" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2442,7 +2771,23 @@
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
-      <c r="L19" s="28" t="s">
+      <c r="L19" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2451,7 +2796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -2805,7 +3150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -3110,7 +3455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Created Some Enemy Prefabs. Created Boss class and SpiderBoss class
Prefabs made for Bandit, Eagle, SpiderBoss, and Wolf

Created Boss class which derives from Enemy
Created SpiderBoss class which derives from Boss

Updated Enemy class to better support Boss class
Created FlyingEnemy class which derives from Enemy
Created StandingEnemy class which derives from Enemy

Updated Task list
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="188">
   <si>
     <t>Feature</t>
   </si>
@@ -556,12 +556,6 @@
     <t>fix any issues with the Finite state machine for the enemy</t>
   </si>
   <si>
-    <t>Create FireSpell Class</t>
-  </si>
-  <si>
-    <t>Create FrostSpell Class</t>
-  </si>
-  <si>
     <t>Alter ComparedItem Class to display equipped Magic</t>
   </si>
   <si>
@@ -572,6 +566,33 @@
   </si>
   <si>
     <t>Fix issue of IconSpawner always spawning FrostBlast Icons</t>
+  </si>
+  <si>
+    <t>Create Prefab for Orc and Skeleton</t>
+  </si>
+  <si>
+    <t>Create Prefab for Moutain Lion</t>
+  </si>
+  <si>
+    <t>Spawn Enemy Prefab depending on the level selected</t>
+  </si>
+  <si>
+    <t>Similar to Bandit</t>
+  </si>
+  <si>
+    <t>Similar to Wolf</t>
+  </si>
+  <si>
+    <t>Create Lightning Magic</t>
+  </si>
+  <si>
+    <t>Create FireBlastMagic Class</t>
+  </si>
+  <si>
+    <t>Create FrostBlastMagic Class</t>
+  </si>
+  <si>
+    <t>Create SpiderBoss Class</t>
   </si>
 </sst>
 </file>
@@ -2068,10 +2089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,6 +2103,7 @@
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
@@ -2112,29 +2134,22 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="14">
-        <v>2</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="25">
+        <v>3</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -2186,7 +2201,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
@@ -2210,7 +2225,7 @@
     </row>
     <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B6" s="14">
         <v>2</v>
@@ -2222,55 +2237,53 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B8" s="14">
-        <f>SUM(B2:B6)</f>
-        <v>13</v>
-      </c>
-      <c r="C8" s="14">
-        <f>SUM(C2:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="14">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
@@ -2287,9 +2300,17 @@
       <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>18.5</v>
+      </c>
+      <c r="C11" s="14">
+        <f>SUM(C3:C10)</f>
+        <v>0</v>
+      </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -2340,9 +2361,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="26" t="s">
-        <v>121</v>
-      </c>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
@@ -2356,9 +2375,7 @@
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="27" t="s">
-        <v>122</v>
-      </c>
+      <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
@@ -2372,7 +2389,53 @@
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="28" t="s">
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2383,10 +2446,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,7 +2493,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B2" s="14">
         <v>1.5</v>
@@ -2438,7 +2501,9 @@
       <c r="C2" s="14">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="14">
+        <v>0.5</v>
+      </c>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
@@ -2454,7 +2519,7 @@
     </row>
     <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B3" s="14">
         <v>1.5</v>
@@ -2462,6 +2527,9 @@
       <c r="C3" s="14">
         <v>2</v>
       </c>
+      <c r="D3" s="14">
+        <v>0.5</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
@@ -2469,7 +2537,7 @@
         <v>123</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2479,13 +2547,17 @@
       <c r="B4" s="14">
         <v>2</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-1</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>122</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>161</v>
@@ -2503,13 +2575,15 @@
       <c r="B5" s="14">
         <v>4</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="14">
+        <v>2</v>
+      </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
+      <c r="F5" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>169</v>
@@ -2527,13 +2601,17 @@
       <c r="B6" s="14">
         <v>3</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="C6" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>-1.5</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>170</v>
@@ -2544,49 +2622,40 @@
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="14">
+        <v>2</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B8" s="14">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>122</v>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2596,13 +2665,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B9" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
@@ -2612,7 +2681,7 @@
         <v>122</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2620,49 +2689,56 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B10" s="14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C10" s="14">
         <v>0.5</v>
       </c>
+      <c r="D10" s="14"/>
       <c r="E10" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-    </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="14">
-        <f>SUM(B2:B10)</f>
-        <v>17.5</v>
-      </c>
-      <c r="C12" s="14">
-        <f>SUM(C2:C11)</f>
-        <v>6</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -2674,9 +2750,17 @@
       <c r="L12" s="14"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>19.5</v>
+      </c>
+      <c r="C13" s="14">
+        <f>SUM(C2:C12)</f>
+        <v>12.5</v>
+      </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -2755,9 +2839,7 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="26" t="s">
-        <v>121</v>
-      </c>
+      <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
@@ -2771,8 +2853,8 @@
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
-      <c r="L19" s="27" t="s">
-        <v>122</v>
+      <c r="L19" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2787,7 +2869,23 @@
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
-      <c r="L20" s="28" t="s">
+      <c r="L20" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="28" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more enemy prefabs, added stand state for enemy and health bars to enemy, added more magic
Added Lightning

Enemies now spawn in depending on level selected

Added RangedEnemy class
Added Archer, Orc, Skeleton, and Cougar prefabs
Added Health Bar to enemy class
Added Enemy tag to enemy prefabs
Added Stand state to enemy class

Shields now use prefabs and enemy attacks are now blocked using
collisons
Shield defence value now displays over shield

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -13,11 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId2"/>
-    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId3"/>
-    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId4"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId5"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId6"/>
+    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId2"/>
+    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId3"/>
+    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId4"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId5"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId6"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="205">
   <si>
     <t>Feature</t>
   </si>
@@ -589,13 +590,61 @@
     <t>Create SpiderBoss Class</t>
   </si>
   <si>
-    <t>Create RangedEnemy class</t>
-  </si>
-  <si>
     <t>Spawn Enemy Prefab into level depending on the level selected</t>
   </si>
   <si>
-    <t>Create Prefab for Mountain Lion</t>
+    <t>Shield works with collisions</t>
+  </si>
+  <si>
+    <t>Shield uses prefab</t>
+  </si>
+  <si>
+    <t>Create Prefab for Cougar</t>
+  </si>
+  <si>
+    <t>Shield Defence text above ShieldControl</t>
+  </si>
+  <si>
+    <t>Upgrade to Unity 5</t>
+  </si>
+  <si>
+    <t>Have Background load in depending on level</t>
+  </si>
+  <si>
+    <t>Incorporate ItemDatabase</t>
+  </si>
+  <si>
+    <t>Create EnemyShot class</t>
+  </si>
+  <si>
+    <t>Prevent shild use after Defence is 0</t>
+  </si>
+  <si>
+    <t>Add Stand state to enemy and improve attack movement</t>
+  </si>
+  <si>
+    <t>Create ImprisonmentMagic</t>
+  </si>
+  <si>
+    <t>Create PoisonMagic</t>
+  </si>
+  <si>
+    <t>Create BarrierMagic</t>
+  </si>
+  <si>
+    <t>Create HealthMagic</t>
+  </si>
+  <si>
+    <t>Use OnCollisionStay for enemies</t>
+  </si>
+  <si>
+    <t>Implement LevelStateManager</t>
+  </si>
+  <si>
+    <t>Create RangedEnemy class and Archer Prefab</t>
+  </si>
+  <si>
+    <t>Have Shield work with enemy projectiles</t>
   </si>
 </sst>
 </file>
@@ -2092,10 +2141,408 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="14">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="14">
+        <v>3</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="14">
+        <v>2</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="14">
+        <f>SUM(B2:B14)</f>
+        <v>18.5</v>
+      </c>
+      <c r="C16" s="14">
+        <f>SUM(C2:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,13 +2591,17 @@
       <c r="B2" s="25">
         <v>3</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="25">
+        <v>1</v>
+      </c>
+      <c r="D2" s="25">
+        <v>-2</v>
+      </c>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G2" s="25"/>
     </row>
@@ -2185,11 +2636,17 @@
       <c r="B4" s="14">
         <v>2</v>
       </c>
+      <c r="C4" s="14">
+        <v>2</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2199,11 +2656,17 @@
       <c r="B5" s="14">
         <v>1</v>
       </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>180</v>
@@ -2211,16 +2674,22 @@
     </row>
     <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B6" s="14">
         <v>0.5</v>
       </c>
+      <c r="C6" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>181</v>
@@ -2228,95 +2697,123 @@
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="14">
         <v>4</v>
       </c>
+      <c r="C7" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="14">
+        <v>-2.5</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>
       </c>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="B10" s="14">
-        <f>SUM(B2:B8)</f>
-        <v>14.5</v>
+        <v>1.5</v>
       </c>
       <c r="C10" s="14">
-        <f>SUM(C3:C9)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="14">
         <v>0</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -2333,9 +2830,17 @@
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="14">
+        <f>SUM(B2:B12)</f>
+        <v>20</v>
+      </c>
+      <c r="C14" s="14">
+        <f>SUM(C2:C13)</f>
+        <v>12.5</v>
+      </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -2372,9 +2877,7 @@
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="26" t="s">
-        <v>121</v>
-      </c>
+      <c r="L16" s="14"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
@@ -2388,9 +2891,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="27" t="s">
-        <v>122</v>
-      </c>
+      <c r="L17" s="14"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
@@ -2404,7 +2905,67 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="28" t="s">
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2413,11 +2974,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -2863,7 +3424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -3217,7 +3778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -3522,7 +4083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added JsonFX, added FireBlastParticles, Updated to Unity 5
Updated to Unity 5

Added JsonFx for serialization and deserialization

Added Serialize method to Inventory

Added FireBlastParticles for magic effects (still in progress)

Added an OnDestory method for Icons

Added GetCurrentState to LevelStateManager to get the level's state

Changed constructor for InventoryItem and its derivatives

Reduced code duplication in the MagicIcon class

Updated InventoryItemDatabase class

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityGames\RPGHeroPrototype\TechnicalDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\UnityGames\RPGHeroPrototype\TechnicalDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16673" windowHeight="6623" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
-    <sheet name="BackLog" sheetId="8" r:id="rId2"/>
-    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId3"/>
-    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId4"/>
-    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId5"/>
-    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId6"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId7"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId8"/>
+    <sheet name="TODO" sheetId="9" r:id="rId2"/>
+    <sheet name="BackLog" sheetId="8" r:id="rId3"/>
+    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId4"/>
+    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId5"/>
+    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId6"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId7"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId8"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="221">
   <si>
     <t>Feature</t>
   </si>
@@ -652,6 +653,48 @@
   </si>
   <si>
     <t>Add Particle Effects to FrostBlast</t>
+  </si>
+  <si>
+    <t>What is left to do</t>
+  </si>
+  <si>
+    <t>Particle effects for magic</t>
+  </si>
+  <si>
+    <t>Inventory Scene</t>
+  </si>
+  <si>
+    <t>Store Scene</t>
+  </si>
+  <si>
+    <t>Enemy animations</t>
+  </si>
+  <si>
+    <t>Load and Save Player</t>
+  </si>
+  <si>
+    <t>Reduced code duplication in MagicIcon class</t>
+  </si>
+  <si>
+    <t>Hours Assigned</t>
+  </si>
+  <si>
+    <t>Total Hours</t>
+  </si>
+  <si>
+    <t>Adjusted size of textures for Unity 5</t>
+  </si>
+  <si>
+    <t>Improved LevelStateManager</t>
+  </si>
+  <si>
+    <t>Can now get current state, enemy stops moving when level is over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update is no longer overriden </t>
+  </si>
+  <si>
+    <t>Result of Unity 5</t>
   </si>
 </sst>
 </file>
@@ -738,11 +781,59 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -751,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -825,6 +916,12 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1117,15 +1214,15 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" customWidth="1"/>
-    <col min="6" max="6" width="255.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="255.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1145,7 +1242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1155,7 +1252,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1272,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="13"/>
       <c r="C4" s="23"/>
@@ -1183,7 +1280,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
@@ -1201,7 +1298,7 @@
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="13" t="s">
         <v>99</v>
@@ -1217,7 +1314,7 @@
       </c>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1227,7 +1324,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
@@ -1247,7 +1344,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1255,7 +1352,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -1275,7 +1372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="10"/>
       <c r="C11" s="17"/>
@@ -1283,7 +1380,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1303,7 +1400,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
@@ -1311,7 +1408,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>81</v>
       </c>
@@ -1331,7 +1428,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
         <v>83</v>
@@ -1349,7 +1446,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
         <v>84</v>
@@ -1367,7 +1464,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15" t="s">
         <v>85</v>
@@ -1385,7 +1482,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="10"/>
       <c r="C18" s="17"/>
@@ -1393,7 +1490,7 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -1413,7 +1510,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="9" t="s">
         <v>97</v>
@@ -1431,7 +1528,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
@@ -1441,7 +1538,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1461,7 +1558,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="9" t="s">
         <v>63</v>
@@ -1479,7 +1576,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="9" t="s">
         <v>64</v>
@@ -1497,7 +1594,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1505,7 +1602,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>71</v>
       </c>
@@ -1525,7 +1622,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="9" t="s">
         <v>72</v>
@@ -1543,7 +1640,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="9" t="s">
         <v>90</v>
@@ -1561,7 +1658,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="10"/>
       <c r="C30" s="17"/>
@@ -1569,7 +1666,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>65</v>
       </c>
@@ -1589,7 +1686,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="9" t="s">
         <v>67</v>
@@ -1607,7 +1704,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="9" t="s">
         <v>68</v>
@@ -1625,7 +1722,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="9" t="s">
         <v>70</v>
@@ -1643,7 +1740,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="9" t="s">
         <v>69</v>
@@ -1661,7 +1758,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="10" t="s">
         <v>107</v>
@@ -1679,7 +1776,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -1687,7 +1784,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>109</v>
       </c>
@@ -1699,7 +1796,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>110</v>
@@ -1709,7 +1806,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>112</v>
@@ -1719,7 +1816,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -1727,7 +1824,7 @@
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>113</v>
       </c>
@@ -1737,7 +1834,7 @@
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -1745,7 +1842,7 @@
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
     </row>
-    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>114</v>
       </c>
@@ -1757,7 +1854,7 @@
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
     </row>
-    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>116</v>
@@ -1767,7 +1864,7 @@
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>117</v>
@@ -1777,7 +1874,7 @@
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
     </row>
-    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>118</v>
@@ -1787,7 +1884,7 @@
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -1795,7 +1892,7 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>11</v>
       </c>
@@ -1805,7 +1902,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>13</v>
       </c>
@@ -1825,7 +1922,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="9" t="s">
         <v>41</v>
@@ -1843,7 +1940,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="9" t="s">
         <v>44</v>
@@ -1861,7 +1958,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="9" t="s">
         <v>45</v>
@@ -1879,7 +1976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="9" t="s">
         <v>46</v>
@@ -1897,7 +1994,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="9" t="s">
         <v>47</v>
@@ -1913,7 +2010,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="10"/>
       <c r="C56" s="17"/>
@@ -1921,7 +2018,7 @@
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>14</v>
       </c>
@@ -1941,7 +2038,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -1949,7 +2046,7 @@
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>15</v>
       </c>
@@ -1969,7 +2066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="14" t="s">
         <v>54</v>
@@ -1987,11 +2084,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
       <c r="B61" s="24"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>16</v>
       </c>
@@ -2001,7 +2098,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>17</v>
       </c>
@@ -2021,7 +2118,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="9" t="s">
         <v>19</v>
@@ -2039,7 +2136,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="9" t="s">
         <v>20</v>
@@ -2057,7 +2154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="9" t="s">
         <v>33</v>
@@ -2075,7 +2172,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="15" t="s">
         <v>31</v>
@@ -2093,7 +2190,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17"/>
       <c r="B68" s="15" t="s">
         <v>32</v>
@@ -2111,7 +2208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17"/>
       <c r="B69" s="15" t="s">
         <v>34</v>
@@ -2129,7 +2226,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C71" s="14"/>
       <c r="D71" s="20" t="s">
         <v>21</v>
@@ -2148,177 +2245,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="42.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.796875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B2" s="14">
-        <v>2</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="B5" s="14">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B6" s="14">
-        <v>3</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="B7" s="14">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="B8" s="14">
-        <v>2</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>206</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>121</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2328,24 +2295,203 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="14">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="14">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2373,21 +2519,27 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>191</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
       </c>
+      <c r="C2" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="14">
+        <v>-0.5</v>
+      </c>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F2" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>192</v>
       </c>
@@ -2401,21 +2553,24 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>193</v>
       </c>
       <c r="B4" s="14">
         <v>6</v>
       </c>
+      <c r="C4" s="14">
+        <v>5.5</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F4" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>203</v>
       </c>
@@ -2429,7 +2584,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>204</v>
       </c>
@@ -2443,21 +2598,24 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>205</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
       </c>
+      <c r="C7" s="14">
+        <v>2.5</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F7" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>201</v>
       </c>
@@ -2471,43 +2629,534 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="14">
+    <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" s="14">
         <f>SUM(B2:B8)</f>
         <v>14</v>
       </c>
+      <c r="C13" s="14">
+        <f>SUM(C2:C12)</f>
+        <v>10</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B2:B11)</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L21:L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="25">
+        <v>3</v>
+      </c>
+      <c r="C2" s="25">
+        <v>1</v>
+      </c>
+      <c r="D2" s="25">
+        <v>-2</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="14">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="14">
+        <v>-2.5</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1.5</v>
+      </c>
       <c r="C10" s="14">
-        <f>SUM(C2:C9)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="14">
         <v>0</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="14">
+        <f>SUM(B2:B12)</f>
+        <v>20</v>
+      </c>
+      <c r="C14" s="14">
+        <f>SUM(C2:C13)</f>
+        <v>12.5</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -2521,7 +3170,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -2535,7 +3184,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -2549,7 +3198,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -2563,422 +3212,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-    </row>
-    <row r="22" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="25">
-        <v>3</v>
-      </c>
-      <c r="C2" s="25">
-        <v>1</v>
-      </c>
-      <c r="D2" s="25">
-        <v>-2</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="14">
-        <v>2</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
-        <v>2</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B5" s="14">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14">
-        <v>1</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="B7" s="14">
-        <v>4</v>
-      </c>
-      <c r="C7" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D7" s="14">
-        <v>-2.5</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" s="14">
-        <v>2</v>
-      </c>
-      <c r="C8" s="14">
-        <v>2</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="C9" s="14">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14">
-        <v>-0.5</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="C10" s="14">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14">
-        <v>-0.5</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="B12" s="14">
-        <v>2</v>
-      </c>
-      <c r="C12" s="14">
-        <v>2</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="14">
-        <f>SUM(B2:B12)</f>
-        <v>20</v>
-      </c>
-      <c r="C14" s="14">
-        <f>SUM(C2:C13)</f>
-        <v>12.5</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -2994,7 +3228,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -3010,7 +3244,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -3031,7 +3265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
@@ -3039,18 +3273,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.73046875" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3078,7 +3312,7 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>183</v>
       </c>
@@ -3104,7 +3338,7 @@
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>184</v>
       </c>
@@ -3127,7 +3361,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>156</v>
       </c>
@@ -3155,7 +3389,7 @@
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>155</v>
       </c>
@@ -3181,7 +3415,7 @@
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>157</v>
       </c>
@@ -3209,7 +3443,7 @@
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>185</v>
       </c>
@@ -3226,7 +3460,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>175</v>
       </c>
@@ -3250,7 +3484,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>174</v>
       </c>
@@ -3276,7 +3510,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>173</v>
       </c>
@@ -3302,7 +3536,7 @@
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>178</v>
       </c>
@@ -3322,7 +3556,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -3336,7 +3570,7 @@
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>120</v>
       </c>
@@ -3358,7 +3592,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -3372,7 +3606,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -3386,7 +3620,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -3400,7 +3634,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -3414,7 +3648,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -3428,7 +3662,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -3444,7 +3678,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -3460,7 +3694,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -3481,7 +3715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -3489,16 +3723,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3522,7 +3756,7 @@
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>154</v>
       </c>
@@ -3540,7 +3774,7 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>152</v>
       </c>
@@ -3562,7 +3796,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>160</v>
       </c>
@@ -3586,7 +3820,7 @@
       </c>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>156</v>
       </c>
@@ -3603,7 +3837,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>155</v>
       </c>
@@ -3617,7 +3851,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>157</v>
       </c>
@@ -3631,7 +3865,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>131</v>
       </c>
@@ -3650,7 +3884,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>159</v>
       </c>
@@ -3670,7 +3904,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>166</v>
       </c>
@@ -3687,7 +3921,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>165</v>
       </c>
@@ -3707,7 +3941,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>163</v>
       </c>
@@ -3727,7 +3961,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>164</v>
       </c>
@@ -3747,7 +3981,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>167</v>
       </c>
@@ -3767,7 +4001,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>172</v>
       </c>
@@ -3787,7 +4021,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -3797,7 +4031,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>120</v>
       </c>
@@ -3815,17 +4049,17 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L23" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L24" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L25" s="28" t="s">
         <v>123</v>
       </c>
@@ -3835,7 +4069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -3843,16 +4077,16 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.265625" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3875,7 +4109,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>151</v>
       </c>
@@ -3896,7 +4130,7 @@
       </c>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>142</v>
       </c>
@@ -3917,7 +4151,7 @@
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>143</v>
       </c>
@@ -3940,7 +4174,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>144</v>
       </c>
@@ -3961,7 +4195,7 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>152</v>
       </c>
@@ -3978,7 +4212,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>145</v>
       </c>
@@ -4001,7 +4235,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>148</v>
       </c>
@@ -4024,7 +4258,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>146</v>
       </c>
@@ -4050,7 +4284,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>131</v>
       </c>
@@ -4072,7 +4306,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>150</v>
       </c>
@@ -4092,7 +4326,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>153</v>
       </c>
@@ -4109,7 +4343,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -4118,7 +4352,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>120</v>
       </c>
@@ -4140,7 +4374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
@@ -4148,19 +4382,19 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.73046875" customWidth="1"/>
-    <col min="3" max="3" width="14.1328125" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.73046875" customWidth="1"/>
-    <col min="13" max="13" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -4183,7 +4417,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -4203,7 +4437,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>125</v>
       </c>
@@ -4226,7 +4460,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -4246,7 +4480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -4269,7 +4503,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -4289,7 +4523,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -4309,7 +4543,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4332,7 +4566,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -4358,7 +4592,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -4381,7 +4615,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -4407,7 +4641,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -4427,7 +4661,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -4447,7 +4681,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -4470,7 +4704,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Filled in ItemDatabase.json, Incorporated InventoryItemDatabase
ItemDatabase.json contains all items in the game

Player's inventory now gets items from the InventoryItemDatabase

Database class added as a wrapper for the list class

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="231">
   <si>
     <t>Feature</t>
   </si>
@@ -613,9 +613,6 @@
     <t>Have Background load in depending on level</t>
   </si>
   <si>
-    <t>Incorporate ItemDatabase</t>
-  </si>
-  <si>
     <t>Add Stand state to enemy and improve attack movement</t>
   </si>
   <si>
@@ -658,9 +655,6 @@
     <t>What is left to do</t>
   </si>
   <si>
-    <t>Particle effects for magic</t>
-  </si>
-  <si>
     <t>Inventory Scene</t>
   </si>
   <si>
@@ -670,9 +664,6 @@
     <t>Enemy animations</t>
   </si>
   <si>
-    <t>Load and Save Player</t>
-  </si>
-  <si>
     <t>Reduced code duplication in MagicIcon class</t>
   </si>
   <si>
@@ -695,6 +686,45 @@
   </si>
   <si>
     <t>Result of Unity 5</t>
+  </si>
+  <si>
+    <t>Audio for the entire game</t>
+  </si>
+  <si>
+    <t>Particle effects for all magic</t>
+  </si>
+  <si>
+    <t>Load and Save Player stats and inventory</t>
+  </si>
+  <si>
+    <t>Going to use Free sounds</t>
+  </si>
+  <si>
+    <t>Currently about 60% complete</t>
+  </si>
+  <si>
+    <t>Will be able to re use a lot of the inventory</t>
+  </si>
+  <si>
+    <t>Will be easier to achieve once the InventoryItemDatabase is working</t>
+  </si>
+  <si>
+    <t>Player leveling up</t>
+  </si>
+  <si>
+    <t>Player stats being taken into effect</t>
+  </si>
+  <si>
+    <t>Challenging</t>
+  </si>
+  <si>
+    <t>Boss Enemies and their special attacks</t>
+  </si>
+  <si>
+    <t>Fix issue that causes enemies to be unkillable</t>
+  </si>
+  <si>
+    <t>Incorporate InventoryItemDatabase</t>
   </si>
 </sst>
 </file>
@@ -842,7 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -922,6 +952,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2245,47 +2276,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>212</v>
+      <c r="B9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2353,7 +2423,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
@@ -2370,7 +2440,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4" s="14">
         <v>1</v>
@@ -2387,7 +2457,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5" s="14">
         <v>1</v>
@@ -2404,7 +2474,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B6" s="14">
         <v>3</v>
@@ -2421,7 +2491,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" s="14">
         <v>1</v>
@@ -2438,7 +2508,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>
@@ -2455,7 +2525,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2474,10 +2544,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,24 +2625,27 @@
     </row>
     <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>193</v>
+        <v>230</v>
       </c>
       <c r="B4" s="14">
         <v>6</v>
       </c>
       <c r="C4" s="14">
-        <v>5.5</v>
+        <v>9.5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3.5</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>122</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5" s="14">
         <v>1.5</v>
@@ -2586,7 +2659,7 @@
     </row>
     <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="14">
         <v>0.5</v>
@@ -2600,7 +2673,7 @@
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
@@ -2617,7 +2690,7 @@
     </row>
     <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B8" s="14">
         <v>1.5</v>
@@ -2631,7 +2704,7 @@
     </row>
     <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B9" s="32">
         <v>0.5</v>
@@ -2647,12 +2720,12 @@
         <v>123</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B10" s="29">
         <v>0.5</v>
@@ -2668,12 +2741,12 @@
         <v>123</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B11" s="29">
         <v>0.5</v>
@@ -2689,35 +2762,29 @@
         <v>123</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="B13" s="14">
-        <f>SUM(B2:B8)</f>
-        <v>14</v>
-      </c>
-      <c r="C13" s="14">
-        <f>SUM(C2:C12)</f>
-        <v>10</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -2729,27 +2796,35 @@
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="B14">
-        <f>SUM(B2:B11)</f>
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="14">
+        <f>SUM(B2:B8)</f>
+        <v>14</v>
+      </c>
+      <c r="C14" s="14">
+        <f>SUM(C2:C13)</f>
+        <v>14</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B2:B12)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
@@ -2760,9 +2835,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="27" t="s">
-        <v>122</v>
-      </c>
+      <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
@@ -2776,8 +2849,8 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="28" t="s">
-        <v>123</v>
+      <c r="I21" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
@@ -2792,7 +2865,9 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
+      <c r="I22" s="28" t="s">
+        <v>123</v>
+      </c>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
@@ -2812,17 +2887,31 @@
       <c r="L23" s="14"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+    </row>
     <row r="26" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3008,7 +3097,7 @@
     </row>
     <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>
@@ -3088,7 +3177,7 @@
     </row>
     <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="14">
         <v>2</v>

</xml_diff>

<commit_message>
Background loads in based on the section
The background now loads in based on the section

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -2368,13 +2368,13 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2547,7 +2547,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2597,10 +2597,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="14">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>106</v>
@@ -2616,11 +2613,14 @@
       <c r="B3" s="14">
         <v>1.5</v>
       </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="C14" s="14">
         <f>SUM(C2:C13)</f>
-        <v>14</v>
+        <v>15.5</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>

</xml_diff>

<commit_message>
Updated FlyingEnemy class and Task List
FlyingEnemy now "Flys"

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="254">
   <si>
     <t>Feature</t>
   </si>
@@ -629,9 +629,6 @@
     <t>Create HealthMagic</t>
   </si>
   <si>
-    <t>Implement LevelStateManager</t>
-  </si>
-  <si>
     <t>Create RangedEnemy class and Archer Prefab</t>
   </si>
   <si>
@@ -647,9 +644,6 @@
     <t>Improve Collision(change to OnEnterStay)</t>
   </si>
   <si>
-    <t>Add Particle effects to FireBlast</t>
-  </si>
-  <si>
     <t>Inventory Scene</t>
   </si>
   <si>
@@ -686,30 +680,15 @@
     <t>Audio for the entire game</t>
   </si>
   <si>
-    <t>Particle effects for all magic</t>
-  </si>
-  <si>
     <t>Load and Save Player stats and inventory</t>
   </si>
   <si>
-    <t>Going to use Free sounds</t>
-  </si>
-  <si>
-    <t>Currently about 60% complete</t>
-  </si>
-  <si>
     <t>Will be able to re use a lot of the inventory</t>
   </si>
   <si>
-    <t>Will be easier to achieve once the InventoryItemDatabase is working</t>
-  </si>
-  <si>
     <t>Player stats being taken into effect</t>
   </si>
   <si>
-    <t>Challenging</t>
-  </si>
-  <si>
     <t>Boss Enemies and their special attacks</t>
   </si>
   <si>
@@ -734,10 +713,88 @@
     <t>Player leveling up(player being able to control their stats)</t>
   </si>
   <si>
-    <t>Proper Level State Management</t>
-  </si>
-  <si>
     <t>Had to remove the methods from the events</t>
+  </si>
+  <si>
+    <t>Implement Saving and Loading of Player class</t>
+  </si>
+  <si>
+    <t>Add UI Sound Effects</t>
+  </si>
+  <si>
+    <t>Have FlyingEnemy fly</t>
+  </si>
+  <si>
+    <t>Have Inventory Serialized before Deserialization</t>
+  </si>
+  <si>
+    <t>Create Temporary Coin holding</t>
+  </si>
+  <si>
+    <t>Particle effects for all magic and enemies</t>
+  </si>
+  <si>
+    <t>UI, Magic, Enemy sounds, (Going to use Free sounds)</t>
+  </si>
+  <si>
+    <t>Currently about 60% complete (need to implement comparison of equipped magic)</t>
+  </si>
+  <si>
+    <t>Create more Weapons and shields</t>
+  </si>
+  <si>
+    <t>Have Icons move with IconSlots and be able to pause icon movement</t>
+  </si>
+  <si>
+    <t>Add Particle effects to FireBlast and FrostBlast</t>
+  </si>
+  <si>
+    <t>Fix Icons Stopping when thrown</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t>Save Player stats and Inventory</t>
+  </si>
+  <si>
+    <t>Allow player to increase their stats</t>
+  </si>
+  <si>
+    <t>Mana and Stamina costs reflected by Player stats</t>
+  </si>
+  <si>
+    <t>Move, attack, die</t>
+  </si>
+  <si>
+    <t>Magic and Weapons being more or less effective against enemies</t>
+  </si>
+  <si>
+    <t>Finishing enemies</t>
+  </si>
+  <si>
+    <t>Bear, Polar Bear</t>
+  </si>
+  <si>
+    <t>Combat System</t>
+  </si>
+  <si>
+    <t>Added State to IconSpawner</t>
+  </si>
+  <si>
+    <t>Fix Shield Issue</t>
+  </si>
+  <si>
+    <t>where shield is being used even when not selected</t>
+  </si>
+  <si>
+    <t>In order to not collect coins if the Player losses the level</t>
+  </si>
+  <si>
+    <t>This way the json file can be altered without having to go into the file and change things manually</t>
+  </si>
+  <si>
+    <t>Sometimes Icons will stop moving when they are thrown</t>
   </si>
 </sst>
 </file>
@@ -885,7 +942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -966,6 +1023,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2638,109 +2697,173 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="36">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" t="s">
         <v>216</v>
       </c>
-      <c r="B2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C7" s="36">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="36">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>217</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" t="s">
+        <v>243</v>
+      </c>
+      <c r="C11" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" s="36">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>218</v>
-      </c>
-      <c r="B6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B8" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>207</v>
-      </c>
-      <c r="B9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>231</v>
+      <c r="B13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C13" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" s="36">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2795,7 +2918,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
@@ -2879,28 +3002,28 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="14">
-        <v>2</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="A8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
@@ -2908,19 +3031,42 @@
       <c r="F9" s="26" t="s">
         <v>121</v>
       </c>
+      <c r="G9" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>121</v>
+      </c>
+      <c r="G10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2930,15 +3076,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -2971,7 +3117,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" s="14">
         <v>1.5</v>
@@ -2990,7 +3136,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3" s="14">
         <v>0.5</v>
@@ -3009,100 +3155,95 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
-        <v>2.5</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>122</v>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="B5" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+      <c r="A6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="B7" s="14">
-        <f>SUM(B2:B5)</f>
-        <v>5.5</v>
-      </c>
-      <c r="C7" s="14">
-        <f>SUM(C2:C6)</f>
-        <v>2.5</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="A7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="B8" s="14">
-        <f>SUM(B2:B5)</f>
-        <v>5.5</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="A8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
@@ -3116,9 +3257,17 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>13.5</v>
+      </c>
+      <c r="C11" s="14">
+        <f>SUM(C2:C10)</f>
+        <v>0</v>
+      </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -3127,8 +3276,13 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>13.5</v>
+      </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -3157,9 +3311,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="27" t="s">
-        <v>122</v>
-      </c>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
@@ -3170,7 +3322,53 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3181,10 +3379,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I22"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3262,7 +3460,7 @@
     </row>
     <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B4" s="14">
         <v>6</v>
@@ -3282,7 +3480,7 @@
     </row>
     <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" s="14">
         <v>1.5</v>
@@ -3296,7 +3494,7 @@
     </row>
     <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" s="14">
         <v>0.5</v>
@@ -3310,7 +3508,7 @@
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>204</v>
+        <v>237</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
@@ -3321,13 +3519,13 @@
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="27" t="s">
-        <v>122</v>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B8" s="14">
         <v>1.5</v>
@@ -3341,7 +3539,7 @@
     </row>
     <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B9" s="32">
         <v>0.5</v>
@@ -3357,12 +3555,12 @@
         <v>123</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B10" s="29">
         <v>0.5</v>
@@ -3378,12 +3576,12 @@
         <v>123</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B11" s="29">
         <v>0.5</v>
@@ -3399,12 +3597,12 @@
         <v>123</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B12" s="29">
         <v>0.5</v>
@@ -3420,35 +3618,29 @@
         <v>123</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B13" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" s="14">
-        <f>SUM(B2:B8)</f>
-        <v>14</v>
-      </c>
-      <c r="C14" s="14">
-        <f>SUM(C2:C13)</f>
-        <v>16.5</v>
-      </c>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -3460,27 +3652,35 @@
       <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="B15">
-        <f>SUM(B2:B12)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
+      <c r="A15" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="14">
+        <f>SUM(B2:B8)</f>
+        <v>14</v>
+      </c>
+      <c r="C15" s="14">
+        <f>SUM(C2:C14)</f>
+        <v>16.5</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16">
+        <f>SUM(B2:B13)</f>
+        <v>16.5</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
@@ -3491,9 +3691,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="27" t="s">
-        <v>122</v>
-      </c>
+      <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
@@ -3507,8 +3705,8 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="28" t="s">
-        <v>123</v>
+      <c r="I22" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
@@ -3523,7 +3721,9 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
+      <c r="I23" s="28" t="s">
+        <v>123</v>
+      </c>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -3543,17 +3743,31 @@
       <c r="L24" s="14"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
     </row>
-    <row r="26" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+    </row>
     <row r="27" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3739,7 +3953,7 @@
     </row>
     <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>

</xml_diff>

<commit_message>
Added SoundManager, Added Background music to all scenes and some UI Sounds, Updated EnemySpawner and IconSpawner, added ability to stop ico
Added SoundManager to manage UI Sounds and Background music

IconSpawner now has a reference to all IconSlots in the scene

Icons, IconSlots, and IconSpawner can now be stopped or paused.

Icons now move based on iconSlot when in Rotating state

Moved code from EnemySpawner and IconSpawner to correct methods

Added OnTriggerStay to enemy class

Fixed Issue with continuous SpiderShot prefabs being instantiated

Fixed Issue of Shield being used even when not selected

Added Base Projectile class

Removed comments from some classes

Reduced code duplication in RangedIcon class

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityGames\RPGHeroPrototype\TechnicalDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\UnityGames\RPGHeroPrototype\TechnicalDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="257">
   <si>
     <t>Feature</t>
   </si>
@@ -719,9 +719,6 @@
     <t>Implement Saving and Loading of Player class</t>
   </si>
   <si>
-    <t>Add UI Sound Effects</t>
-  </si>
-  <si>
     <t>Have FlyingEnemy fly</t>
   </si>
   <si>
@@ -770,18 +767,9 @@
     <t>Magic and Weapons being more or less effective against enemies</t>
   </si>
   <si>
-    <t>Finishing enemies</t>
-  </si>
-  <si>
-    <t>Bear, Polar Bear</t>
-  </si>
-  <si>
     <t>Combat System</t>
   </si>
   <si>
-    <t>Added State to IconSpawner</t>
-  </si>
-  <si>
     <t>Fix Shield Issue</t>
   </si>
   <si>
@@ -795,6 +783,27 @@
   </si>
   <si>
     <t>Sometimes Icons will stop moving when they are thrown</t>
+  </si>
+  <si>
+    <t>Move Start, Running, Won, and Lost code into correct methods</t>
+  </si>
+  <si>
+    <t>Create InventoryItem Prefab for InventoryScene</t>
+  </si>
+  <si>
+    <t>The Prefab will have an image and a description</t>
+  </si>
+  <si>
+    <t>Fix Stopping StandingEnemy issue</t>
+  </si>
+  <si>
+    <t>Time Estimate (in hours)</t>
+  </si>
+  <si>
+    <t>Improve Collision(change to OnTriggerStay2D)</t>
+  </si>
+  <si>
+    <t>Add UI Sound Effects and background music</t>
   </si>
 </sst>
 </file>
@@ -1317,15 +1326,15 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" customWidth="1"/>
-    <col min="6" max="6" width="255.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="255.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1355,7 +1364,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1384,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="13"/>
       <c r="C4" s="23"/>
@@ -1383,7 +1392,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
@@ -1401,7 +1410,7 @@
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="13" t="s">
         <v>99</v>
@@ -1417,7 +1426,7 @@
       </c>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1427,7 +1436,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
@@ -1447,7 +1456,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1455,7 +1464,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -1475,7 +1484,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="10"/>
       <c r="C11" s="17"/>
@@ -1483,7 +1492,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1503,7 +1512,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
@@ -1511,7 +1520,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>81</v>
       </c>
@@ -1531,7 +1540,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
         <v>83</v>
@@ -1549,7 +1558,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
         <v>84</v>
@@ -1567,7 +1576,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15" t="s">
         <v>85</v>
@@ -1585,7 +1594,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="10"/>
       <c r="C18" s="17"/>
@@ -1593,7 +1602,7 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -1613,7 +1622,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="9" t="s">
         <v>97</v>
@@ -1631,7 +1640,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
@@ -1641,7 +1650,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1661,7 +1670,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="9" t="s">
         <v>63</v>
@@ -1679,7 +1688,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="9" t="s">
         <v>64</v>
@@ -1697,7 +1706,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1705,7 +1714,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>71</v>
       </c>
@@ -1725,7 +1734,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="9" t="s">
         <v>72</v>
@@ -1743,7 +1752,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="9" t="s">
         <v>90</v>
@@ -1761,7 +1770,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="10"/>
       <c r="C30" s="17"/>
@@ -1769,7 +1778,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>65</v>
       </c>
@@ -1789,7 +1798,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="9" t="s">
         <v>67</v>
@@ -1807,7 +1816,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="9" t="s">
         <v>68</v>
@@ -1825,7 +1834,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="9" t="s">
         <v>70</v>
@@ -1843,7 +1852,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="9" t="s">
         <v>69</v>
@@ -1861,7 +1870,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="10" t="s">
         <v>107</v>
@@ -1879,7 +1888,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -1887,7 +1896,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>109</v>
       </c>
@@ -1899,7 +1908,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>110</v>
@@ -1909,7 +1918,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>112</v>
@@ -1919,7 +1928,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -1927,7 +1936,7 @@
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>113</v>
       </c>
@@ -1937,7 +1946,7 @@
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -1945,7 +1954,7 @@
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
     </row>
-    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>114</v>
       </c>
@@ -1957,7 +1966,7 @@
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
     </row>
-    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>116</v>
@@ -1967,7 +1976,7 @@
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>117</v>
@@ -1977,7 +1986,7 @@
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
     </row>
-    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>118</v>
@@ -1987,7 +1996,7 @@
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -1995,7 +2004,7 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>11</v>
       </c>
@@ -2005,7 +2014,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>13</v>
       </c>
@@ -2025,7 +2034,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="9" t="s">
         <v>41</v>
@@ -2043,7 +2052,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="9" t="s">
         <v>44</v>
@@ -2061,7 +2070,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="9" t="s">
         <v>45</v>
@@ -2079,7 +2088,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="9" t="s">
         <v>46</v>
@@ -2097,7 +2106,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="9" t="s">
         <v>47</v>
@@ -2113,7 +2122,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="10"/>
       <c r="C56" s="17"/>
@@ -2121,7 +2130,7 @@
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>14</v>
       </c>
@@ -2141,7 +2150,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -2149,7 +2158,7 @@
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>15</v>
       </c>
@@ -2169,7 +2178,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="14" t="s">
         <v>54</v>
@@ -2187,11 +2196,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
       <c r="B61" s="24"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>16</v>
       </c>
@@ -2201,7 +2210,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>17</v>
       </c>
@@ -2221,7 +2230,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="9" t="s">
         <v>19</v>
@@ -2239,7 +2248,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="9" t="s">
         <v>20</v>
@@ -2257,7 +2266,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="9" t="s">
         <v>33</v>
@@ -2275,7 +2284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="15" t="s">
         <v>31</v>
@@ -2293,7 +2302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17"/>
       <c r="B68" s="15" t="s">
         <v>32</v>
@@ -2311,7 +2320,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17"/>
       <c r="B69" s="15" t="s">
         <v>34</v>
@@ -2329,7 +2338,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C71" s="14"/>
       <c r="D71" s="20" t="s">
         <v>21</v>
@@ -2354,19 +2363,19 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.73046875" customWidth="1"/>
-    <col min="3" max="3" width="14.1328125" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.73046875" customWidth="1"/>
-    <col min="13" max="13" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2389,7 +2398,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -2409,7 +2418,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>125</v>
       </c>
@@ -2432,7 +2441,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -2452,7 +2461,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -2475,7 +2484,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -2495,7 +2504,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -2515,7 +2524,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -2538,7 +2547,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -2564,7 +2573,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -2587,7 +2596,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -2613,7 +2622,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -2633,7 +2642,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -2653,7 +2662,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -2676,7 +2685,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -2697,20 +2706,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>221</v>
       </c>
@@ -2718,94 +2728,118 @@
         <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>238</v>
+      </c>
+      <c r="D1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="36">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C3" s="36">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>246</v>
+      <c r="D3" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>231</v>
       </c>
       <c r="C4" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.1</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>203</v>
+      </c>
+      <c r="B5" t="s">
+        <v>233</v>
       </c>
       <c r="C5" s="36">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.6</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="C6" s="36">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.4</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="C7" s="36">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="B8" t="s">
         <v>240</v>
       </c>
       <c r="C8" s="36">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B9" t="s">
         <v>241</v>
       </c>
       <c r="C9" s="36">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B10" t="s">
         <v>242</v>
@@ -2813,42 +2847,37 @@
       <c r="C10" s="36">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>205</v>
-      </c>
-      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" t="s">
         <v>243</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C12" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>218</v>
-      </c>
-      <c r="C12" s="36">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>224</v>
-      </c>
-      <c r="B13" t="s">
         <v>244</v>
       </c>
       <c r="C13" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>247</v>
-      </c>
-      <c r="C14" s="36">
         <v>0.8</v>
       </c>
     </row>
@@ -2860,21 +2889,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2897,12 +2926,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="B2" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -2912,13 +2941,11 @@
       <c r="F2" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
@@ -2933,9 +2960,9 @@
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B4" s="14">
         <v>1</v>
@@ -2950,12 +2977,12 @@
       </c>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B5" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2967,12 +2994,12 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B6" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2984,29 +3011,29 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" s="14">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F7" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>230</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
@@ -3015,12 +3042,12 @@
         <v>121</v>
       </c>
       <c r="G8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3032,41 +3059,21 @@
         <v>121</v>
       </c>
       <c r="G9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="G10" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>238</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3076,23 +3083,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3115,45 +3122,51 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>201</v>
       </c>
       <c r="B2" s="14">
         <v>1.5</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="14">
+        <v>0.5</v>
+      </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
+      <c r="F2" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="B3" s="14">
         <v>1.5</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="14">
+        <v>-1</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>199</v>
       </c>
@@ -3165,28 +3178,34 @@
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
+      <c r="F4" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>222</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>-0.5</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F5" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>223</v>
       </c>
@@ -3200,7 +3219,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>227</v>
       </c>
@@ -3214,95 +3233,123 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="D8">
+        <v>-0.5</v>
+      </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2</v>
+      </c>
+      <c r="C9" s="14">
+        <v>4</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="14">
+        <v>-1.5</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G8" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="B9" s="14">
-        <v>2</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" s="14">
-        <f>SUM(B2:B9)</f>
-        <v>14.5</v>
-      </c>
-      <c r="C11" s="14">
-        <f>SUM(C2:C10)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="31" t="s">
-        <v>208</v>
+      <c r="G11" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>175</v>
       </c>
       <c r="B12" s="14">
-        <f>SUM(B2:B9)</f>
-        <v>14.5</v>
+        <v>2</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="29">
+        <v>2</v>
+      </c>
+      <c r="C13" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="29">
+        <v>-1.5</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -3313,10 +3360,18 @@
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="14">
+        <f>SUM(B2:B12)</f>
+        <v>20.5</v>
+      </c>
+      <c r="C15" s="14">
+        <f>SUM(C2:C14)</f>
+        <v>8</v>
+      </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -3324,9 +3379,14 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="14">
+        <f>SUM(B2:B13)</f>
+        <v>22.5</v>
+      </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -3335,7 +3395,7 @@
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -3346,7 +3406,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -3355,11 +3415,9 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -3368,7 +3426,53 @@
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3385,18 +3489,18 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3424,7 +3528,7 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>191</v>
       </c>
@@ -3441,7 +3545,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>192</v>
       </c>
@@ -3458,7 +3562,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>220</v>
       </c>
@@ -3478,7 +3582,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>201</v>
       </c>
@@ -3492,7 +3596,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>202</v>
       </c>
@@ -3506,9 +3610,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
@@ -3523,7 +3627,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>199</v>
       </c>
@@ -3537,7 +3641,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>209</v>
       </c>
@@ -3558,7 +3662,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>206</v>
       </c>
@@ -3579,7 +3683,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>210</v>
       </c>
@@ -3600,7 +3704,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>219</v>
       </c>
@@ -3621,9 +3725,9 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B13" s="29">
         <v>0.5</v>
@@ -3639,7 +3743,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -3653,7 +3757,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>207</v>
       </c>
@@ -3675,7 +3779,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>208</v>
       </c>
@@ -3684,7 +3788,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -3698,7 +3802,7 @@
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -3714,7 +3818,7 @@
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -3730,7 +3834,7 @@
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -3744,7 +3848,7 @@
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -3758,18 +3862,18 @@
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
     </row>
-    <row r="27" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="29" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="30" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3783,18 +3887,18 @@
       <selection activeCell="L22" sqref="L21:L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3822,7 +3926,7 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>182</v>
       </c>
@@ -3843,7 +3947,7 @@
       </c>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>175</v>
       </c>
@@ -3867,7 +3971,7 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>177</v>
       </c>
@@ -3887,7 +3991,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>179</v>
       </c>
@@ -3910,7 +4014,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>189</v>
       </c>
@@ -3933,7 +4037,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>186</v>
       </c>
@@ -3953,7 +4057,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>198</v>
       </c>
@@ -3973,7 +4077,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>187</v>
       </c>
@@ -3993,7 +4097,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>188</v>
       </c>
@@ -4013,7 +4117,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>190</v>
       </c>
@@ -4033,7 +4137,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>193</v>
       </c>
@@ -4053,7 +4157,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -4067,7 +4171,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>120</v>
       </c>
@@ -4089,7 +4193,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -4103,7 +4207,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -4117,7 +4221,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -4131,7 +4235,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -4145,7 +4249,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -4159,7 +4263,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -4175,7 +4279,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -4191,7 +4295,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -4220,18 +4324,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.73046875" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -4259,7 +4363,7 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>183</v>
       </c>
@@ -4285,7 +4389,7 @@
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>184</v>
       </c>
@@ -4308,7 +4412,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>156</v>
       </c>
@@ -4336,7 +4440,7 @@
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>155</v>
       </c>
@@ -4362,7 +4466,7 @@
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>157</v>
       </c>
@@ -4390,7 +4494,7 @@
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>185</v>
       </c>
@@ -4407,7 +4511,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>175</v>
       </c>
@@ -4431,7 +4535,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>174</v>
       </c>
@@ -4457,7 +4561,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>173</v>
       </c>
@@ -4483,7 +4587,7 @@
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>178</v>
       </c>
@@ -4503,7 +4607,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -4517,7 +4621,7 @@
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>120</v>
       </c>
@@ -4539,7 +4643,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -4553,7 +4657,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -4567,7 +4671,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -4581,7 +4685,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -4595,7 +4699,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -4609,7 +4713,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -4625,7 +4729,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -4641,7 +4745,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -4670,16 +4774,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -4703,7 +4807,7 @@
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>154</v>
       </c>
@@ -4721,7 +4825,7 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>152</v>
       </c>
@@ -4743,7 +4847,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>160</v>
       </c>
@@ -4767,7 +4871,7 @@
       </c>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>156</v>
       </c>
@@ -4784,7 +4888,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>155</v>
       </c>
@@ -4798,7 +4902,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>157</v>
       </c>
@@ -4812,7 +4916,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>131</v>
       </c>
@@ -4831,7 +4935,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>159</v>
       </c>
@@ -4851,7 +4955,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>166</v>
       </c>
@@ -4868,7 +4972,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>165</v>
       </c>
@@ -4888,7 +4992,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>163</v>
       </c>
@@ -4908,7 +5012,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>164</v>
       </c>
@@ -4928,7 +5032,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>167</v>
       </c>
@@ -4948,7 +5052,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>172</v>
       </c>
@@ -4968,7 +5072,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -4978,7 +5082,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>120</v>
       </c>
@@ -4996,17 +5100,17 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L23" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L24" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L25" s="28" t="s">
         <v>123</v>
       </c>
@@ -5024,16 +5128,16 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.265625" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -5056,7 +5160,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>151</v>
       </c>
@@ -5077,7 +5181,7 @@
       </c>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>142</v>
       </c>
@@ -5098,7 +5202,7 @@
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>143</v>
       </c>
@@ -5121,7 +5225,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>144</v>
       </c>
@@ -5142,7 +5246,7 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>152</v>
       </c>
@@ -5159,7 +5263,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>145</v>
       </c>
@@ -5182,7 +5286,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>148</v>
       </c>
@@ -5205,7 +5309,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>146</v>
       </c>
@@ -5231,7 +5335,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>131</v>
       </c>
@@ -5253,7 +5357,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>150</v>
       </c>
@@ -5273,7 +5377,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>153</v>
       </c>
@@ -5290,7 +5394,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -5299,7 +5403,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Player is now saved and loaded, Updated Inventory Scene
Added new game functionality

Player is Saved and Loaded

Inventory Scene works correctly

Created Derived Projectile classes for Arrow and Spider Boss Shot

Fixed Icon Stopping Issue

Created InventoryItemDetails class

Fixed Particles  not showing issue

Fixed Shield being used even when not selected issue

Updated Base Projectile Class

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -15,13 +15,14 @@
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="9" r:id="rId2"/>
     <sheet name="BackLog" sheetId="8" r:id="rId3"/>
-    <sheet name="Tasks 03-11 to 03-18" sheetId="10" r:id="rId4"/>
-    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId5"/>
-    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId6"/>
-    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId7"/>
-    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId8"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId9"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId10"/>
+    <sheet name="Tasks 03-18 to 03-25" sheetId="11" r:id="rId4"/>
+    <sheet name="Tasks 03-11 to 03-18" sheetId="10" r:id="rId5"/>
+    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId6"/>
+    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId7"/>
+    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId8"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId9"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId10"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="270">
   <si>
     <t>Feature</t>
   </si>
@@ -701,109 +702,148 @@
     <t>What is left to do?</t>
   </si>
   <si>
+    <t>Weaknesses implemented into enemies</t>
+  </si>
+  <si>
+    <t>Player leveling up(player being able to control their stats)</t>
+  </si>
+  <si>
+    <t>Had to remove the methods from the events</t>
+  </si>
+  <si>
+    <t>Have FlyingEnemy fly</t>
+  </si>
+  <si>
+    <t>Have Inventory Serialized before Deserialization</t>
+  </si>
+  <si>
+    <t>Create Temporary Coin holding</t>
+  </si>
+  <si>
+    <t>Particle effects for all magic and enemies</t>
+  </si>
+  <si>
+    <t>Create more Weapons and shields</t>
+  </si>
+  <si>
+    <t>Add Particle effects to FireBlast and FrostBlast</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t>Save Player stats and Inventory</t>
+  </si>
+  <si>
+    <t>Allow player to increase their stats</t>
+  </si>
+  <si>
+    <t>Mana and Stamina costs reflected by Player stats</t>
+  </si>
+  <si>
+    <t>Move, attack, die</t>
+  </si>
+  <si>
+    <t>Magic and Weapons being more or less effective against enemies</t>
+  </si>
+  <si>
+    <t>Combat System</t>
+  </si>
+  <si>
+    <t>In order to not collect coins if the Player losses the level</t>
+  </si>
+  <si>
+    <t>This way the json file can be altered without having to go into the file and change things manually</t>
+  </si>
+  <si>
+    <t>Time Estimate (in hours)</t>
+  </si>
+  <si>
+    <t>Add UI Sound Effects and background music</t>
+  </si>
+  <si>
+    <t>Add sound effects to store and Inventory</t>
+  </si>
+  <si>
+    <t>Magic, Enemy sounds</t>
+  </si>
+  <si>
+    <t>Setup InventorySlots in Store Scene to load either Player or clerks inventory</t>
+  </si>
+  <si>
+    <t>Be able to buy or sell selected item in Store Scene</t>
+  </si>
+  <si>
+    <t>Implement Character Level up Screen</t>
+  </si>
+  <si>
+    <t>Fix stopping StandingEnemy</t>
+  </si>
+  <si>
+    <t>Improve Collision(change to OnTriggerStay2D)</t>
+  </si>
+  <si>
     <t>Fix Boss Special Attack spawning issue</t>
   </si>
   <si>
     <t>Fix Particle Stopping</t>
   </si>
   <si>
-    <t>Weaknesses implemented into enemies</t>
-  </si>
-  <si>
-    <t>Player leveling up(player being able to control their stats)</t>
-  </si>
-  <si>
-    <t>Had to remove the methods from the events</t>
-  </si>
-  <si>
     <t>Implement Saving and Loading of Player class</t>
   </si>
   <si>
-    <t>Have FlyingEnemy fly</t>
-  </si>
-  <si>
-    <t>Have Inventory Serialized before Deserialization</t>
-  </si>
-  <si>
-    <t>Create Temporary Coin holding</t>
-  </si>
-  <si>
-    <t>Particle effects for all magic and enemies</t>
-  </si>
-  <si>
-    <t>UI, Magic, Enemy sounds, (Going to use Free sounds)</t>
-  </si>
-  <si>
-    <t>Currently about 60% complete (need to implement comparison of equipped magic)</t>
-  </si>
-  <si>
-    <t>Create more Weapons and shields</t>
-  </si>
-  <si>
     <t>Have Icons move with IconSlots and be able to pause icon movement</t>
   </si>
   <si>
-    <t>Add Particle effects to FireBlast and FrostBlast</t>
-  </si>
-  <si>
-    <t>Fix Icons Stopping when thrown</t>
-  </si>
-  <si>
-    <t>Completion</t>
-  </si>
-  <si>
-    <t>Save Player stats and Inventory</t>
-  </si>
-  <si>
-    <t>Allow player to increase their stats</t>
-  </si>
-  <si>
-    <t>Mana and Stamina costs reflected by Player stats</t>
-  </si>
-  <si>
-    <t>Move, attack, die</t>
-  </si>
-  <si>
-    <t>Magic and Weapons being more or less effective against enemies</t>
-  </si>
-  <si>
-    <t>Combat System</t>
+    <t>Move Start, Running, Won, and Lost code into correct methods</t>
   </si>
   <si>
     <t>Fix Shield Issue</t>
   </si>
   <si>
-    <t>where shield is being used even when not selected</t>
-  </si>
-  <si>
-    <t>In order to not collect coins if the Player losses the level</t>
-  </si>
-  <si>
-    <t>This way the json file can be altered without having to go into the file and change things manually</t>
-  </si>
-  <si>
-    <t>Sometimes Icons will stop moving when they are thrown</t>
-  </si>
-  <si>
-    <t>Move Start, Running, Won, and Lost code into correct methods</t>
-  </si>
-  <si>
-    <t>Create InventoryItem Prefab for InventoryScene</t>
-  </si>
-  <si>
-    <t>The Prefab will have an image and a description</t>
-  </si>
-  <si>
-    <t>Fix Stopping StandingEnemy issue</t>
-  </si>
-  <si>
-    <t>Time Estimate (in hours)</t>
-  </si>
-  <si>
-    <t>Improve Collision(change to OnTriggerStay2D)</t>
-  </si>
-  <si>
-    <t>Add UI Sound Effects and background music</t>
+    <t>Fix Icon appearing below IconSlot</t>
+  </si>
+  <si>
+    <t>Implement Spider Boss Special Attack</t>
+  </si>
+  <si>
+    <t>Shield is used even when not selected</t>
+  </si>
+  <si>
+    <t>Created Derived projectile classes</t>
+  </si>
+  <si>
+    <t>Fixed Stopping Icon issue</t>
+  </si>
+  <si>
+    <t>Icons Stopped when thrown</t>
+  </si>
+  <si>
+    <t>Particles were rendering behind sprite</t>
+  </si>
+  <si>
+    <t>Create InventoryItemDetails Prefab for InventoryScene</t>
+  </si>
+  <si>
+    <t>Add UI Sound Effects</t>
+  </si>
+  <si>
+    <t>Prevent player from selecting shield</t>
+  </si>
+  <si>
+    <t>StandingEnemy moves slightly when they should always be standing</t>
+  </si>
+  <si>
+    <t>Yeti, Giant, and Dragon</t>
+  </si>
+  <si>
+    <t>Special attack was constantly spawning</t>
+  </si>
+  <si>
+    <t>Contains Image and description</t>
+  </si>
+  <si>
+    <t>Alter Inventory Scene to display equipped Magic</t>
   </si>
 </sst>
 </file>
@@ -2357,6 +2397,311 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="25">
+        <v>0</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="14">
+        <v>5</v>
+      </c>
+      <c r="C7" s="14">
+        <v>6</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="14">
+        <v>1</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="14">
+        <f>SUM(B3:B10)</f>
+        <v>14</v>
+      </c>
+      <c r="C14" s="14">
+        <f>SUM(C3:C13)</f>
+        <v>12.75</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2709,7 +3054,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,10 +3073,10 @@
         <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D1" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2739,18 +3084,18 @@
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="C2" s="36">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C3" s="36">
         <v>0</v>
@@ -2761,7 +3106,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C4" s="36">
         <v>0.1</v>
@@ -2774,14 +3119,11 @@
       <c r="A5" t="s">
         <v>203</v>
       </c>
-      <c r="B5" t="s">
-        <v>233</v>
-      </c>
       <c r="C5" s="36">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2792,10 +3134,10 @@
         <v>216</v>
       </c>
       <c r="C6" s="36">
-        <v>0.4</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="14">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2803,21 +3145,21 @@
         <v>215</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C7" s="36">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C8" s="36">
         <v>0.1</v>
@@ -2831,10 +3173,13 @@
         <v>217</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C9" s="36">
         <v>0</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2842,7 +3187,7 @@
         <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C10" s="36">
         <v>0</v>
@@ -2855,8 +3200,11 @@
       <c r="A11" t="s">
         <v>218</v>
       </c>
+      <c r="B11" t="s">
+        <v>266</v>
+      </c>
       <c r="C11" s="36">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="D11">
         <v>20</v>
@@ -2864,21 +3212,27 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C12" s="36">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C13" s="36">
         <v>0.8</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2889,10 +3243,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,7 +3282,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -2945,7 +3299,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
@@ -2962,10 +3316,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B4" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -2979,10 +3333,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B5" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2995,25 +3349,25 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B6" s="14">
-        <v>1</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="A6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F6" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -3025,55 +3379,7 @@
         <v>121</v>
       </c>
       <c r="G7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>230</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>237</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>253</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>121</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3083,9 +3389,202 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="14">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" s="14">
+        <v>5</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="B6" s="14">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="14">
+        <v>8</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="14">
+        <f>SUM(B2:B7)</f>
+        <v>21</v>
+      </c>
+      <c r="C9" s="14">
+        <f>SUM(C2:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" s="14">
+        <f>SUM(B2:B7)</f>
+        <v>21</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -3130,22 +3629,23 @@
         <v>1.5</v>
       </c>
       <c r="C2" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
+        <v>-0.5</v>
+      </c>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="14"/>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
+      </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B3" s="14">
         <v>1.5</v>
@@ -3162,7 +3662,6 @@
       <c r="F3" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
@@ -3173,29 +3672,35 @@
       <c r="B4" s="14">
         <v>1.5</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-0.5</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="14"/>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>258</v>
+      </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="A5" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14">
         <v>0.5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="14">
         <v>-0.5</v>
       </c>
       <c r="E5" s="14" t="s">
@@ -3204,46 +3709,64 @@
       <c r="F5" s="28" t="s">
         <v>123</v>
       </c>
+      <c r="G5" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="A6" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>-0.5</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B7" s="14">
         <v>3</v>
       </c>
+      <c r="C7" s="14">
+        <v>2</v>
+      </c>
+      <c r="D7" s="14">
+        <v>-1</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
+      <c r="A8" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14">
         <v>1.5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="14">
         <v>-0.5</v>
       </c>
       <c r="E8" s="14" t="s">
@@ -3255,7 +3778,7 @@
     </row>
     <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B9" s="14">
         <v>2</v>
@@ -3263,6 +3786,9 @@
       <c r="C9" s="14">
         <v>4</v>
       </c>
+      <c r="D9" s="14">
+        <v>2</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
@@ -3272,7 +3798,7 @@
     </row>
     <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B10" s="14">
         <v>2</v>
@@ -3292,43 +3818,50 @@
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="B11" s="14">
         <v>2</v>
       </c>
+      <c r="C11" s="14">
+        <v>3</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
       <c r="E11" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>121</v>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>175</v>
+        <v>269</v>
       </c>
       <c r="B12" s="14">
         <v>2</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="C12" s="14">
+        <v>3</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
       <c r="E12" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F12" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>140</v>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="B13" s="29">
         <v>2</v>
@@ -3346,147 +3879,247 @@
         <v>123</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" s="14">
-        <f>SUM(B2:B12)</f>
-        <v>20.5</v>
-      </c>
-      <c r="C15" s="14">
-        <f>SUM(C2:C14)</f>
-        <v>8</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B16" s="14">
-        <f>SUM(B2:B13)</f>
-        <v>22.5</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="B14" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="29">
+        <v>2</v>
+      </c>
+      <c r="C15" s="29">
+        <v>2</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="B16" s="29">
+        <v>2</v>
+      </c>
+      <c r="C16" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="29">
+        <v>-1.5</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="G17"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+    </row>
+    <row r="18" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B18" s="14">
+        <f>SUM(B2:B12)</f>
+        <v>20.5</v>
+      </c>
+      <c r="C18" s="14">
+        <f>SUM(C2:C17)</f>
+        <v>22</v>
+      </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="G18"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+    </row>
+    <row r="19" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="14">
+        <f>SUM(B2:B16)</f>
+        <v>27</v>
+      </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="G19"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="28" t="s">
-        <v>123</v>
-      </c>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3612,7 +4245,7 @@
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
@@ -3722,12 +4355,12 @@
         <v>123</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B13" s="29">
         <v>0.5</v>
@@ -3879,7 +4512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
@@ -4316,7 +4949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
@@ -4766,7 +5399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -5118,309 +5751,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="25">
-        <v>0</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14">
-        <v>1</v>
-      </c>
-      <c r="D3" s="14">
-        <v>0</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="14">
-        <v>-0.5</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="14">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B6" s="14">
-        <v>2.5</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" s="14">
-        <v>5</v>
-      </c>
-      <c r="C7" s="14">
-        <v>6</v>
-      </c>
-      <c r="D7" s="14">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C8" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="14">
-        <v>1</v>
-      </c>
-      <c r="C9" s="14">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" s="14">
-        <v>2</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H10" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="C11" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" s="14">
-        <v>1</v>
-      </c>
-      <c r="C12" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="14">
-        <f>SUM(B3:B10)</f>
-        <v>14</v>
-      </c>
-      <c r="C14" s="14">
-        <f>SUM(C3:C13)</f>
-        <v>12.75</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added temp coin storage, shield stops working when defence reaches zero
Coins are only kept if the player wins the level

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="273">
   <si>
     <t>Feature</t>
   </si>
@@ -765,9 +765,6 @@
     <t>Add sound effects to store and Inventory</t>
   </si>
   <si>
-    <t>Magic, Enemy sounds</t>
-  </si>
-  <si>
     <t>Setup InventorySlots in Store Scene to load either Player or clerks inventory</t>
   </si>
   <si>
@@ -844,6 +841,18 @@
   </si>
   <si>
     <t>Alter Inventory Scene to display equipped Magic</t>
+  </si>
+  <si>
+    <t>May need a bit of polish</t>
+  </si>
+  <si>
+    <t>Polish/fix an potential bugs</t>
+  </si>
+  <si>
+    <t>Added enemy burning effect</t>
+  </si>
+  <si>
+    <t>Magic, Enemy sounds, Weapon sounds</t>
   </si>
 </sst>
 </file>
@@ -3053,8 +3062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3084,7 +3093,7 @@
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="C2" s="36">
         <v>0.25</v>
@@ -3101,7 +3110,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="14">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3112,13 +3121,16 @@
         <v>0.1</v>
       </c>
       <c r="D4">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>203</v>
       </c>
+      <c r="B5" t="s">
+        <v>269</v>
+      </c>
       <c r="C5" s="36">
         <v>0.9</v>
       </c>
@@ -3179,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3201,13 +3213,13 @@
         <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C11" s="36">
         <v>0.25</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3227,6 +3239,9 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>237</v>
+      </c>
+      <c r="B13" t="s">
+        <v>270</v>
       </c>
       <c r="C13" s="36">
         <v>0.8</v>
@@ -3243,10 +3258,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,7 +3382,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -3379,7 +3394,21 @@
         <v>121</v>
       </c>
       <c r="G7" t="s">
-        <v>265</v>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3391,8 +3420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3431,7 +3460,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B2" s="14">
         <v>2</v>
@@ -3455,16 +3484,18 @@
       <c r="B3" s="14">
         <v>2</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3474,11 +3505,14 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G4" t="s">
         <v>238</v>
@@ -3486,7 +3520,7 @@
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" s="14">
         <v>5</v>
@@ -3500,7 +3534,7 @@
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B6" s="14">
         <v>3</v>
@@ -3514,7 +3548,7 @@
     </row>
     <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B7" s="14">
         <v>8</v>
@@ -3545,7 +3579,7 @@
       </c>
       <c r="C9" s="14">
         <f>SUM(C2:C8)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -3585,7 +3619,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection sqref="A1:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3645,7 +3679,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3" s="14">
         <v>1.5</v>
@@ -3685,14 +3719,14 @@
         <v>123</v>
       </c>
       <c r="G4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B5" s="14">
         <v>1</v>
@@ -3710,12 +3744,12 @@
         <v>123</v>
       </c>
       <c r="G5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B6" s="14">
         <v>2</v>
@@ -3733,12 +3767,12 @@
         <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B7" s="14">
         <v>3</v>
@@ -3758,7 +3792,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>
@@ -3798,7 +3832,7 @@
     </row>
     <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B10" s="14">
         <v>2</v>
@@ -3818,7 +3852,7 @@
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B11" s="14">
         <v>2</v>
@@ -3836,12 +3870,12 @@
         <v>123</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B12" s="14">
         <v>2</v>
@@ -3861,7 +3895,7 @@
     </row>
     <row r="13" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B13" s="29">
         <v>2</v>
@@ -3879,12 +3913,12 @@
         <v>123</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B14" s="29">
         <v>0.5</v>
@@ -3904,7 +3938,7 @@
     </row>
     <row r="15" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B15" s="29">
         <v>2</v>
@@ -3924,7 +3958,7 @@
     </row>
     <row r="16" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B16" s="29">
         <v>2</v>
@@ -3942,7 +3976,7 @@
         <v>123</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated numerous classes to support store scene
Updated Clerk class
Updated HealthPotion class
Updated InventoryItem class
Updated InventorySlot class
Updated ManaPotion class
Updated Shield class
Updated StoreScript

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="274">
   <si>
     <t>Feature</t>
   </si>
@@ -849,10 +849,13 @@
     <t>Polish/fix an potential bugs</t>
   </si>
   <si>
-    <t>Added enemy burning effect</t>
-  </si>
-  <si>
     <t>Magic, Enemy sounds, Weapon sounds</t>
+  </si>
+  <si>
+    <t>Add Enemy Froze Effect</t>
+  </si>
+  <si>
+    <t>Add Enemy Burning effect</t>
   </si>
 </sst>
 </file>
@@ -3062,8 +3065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3093,7 +3096,7 @@
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C2" s="36">
         <v>0.25</v>
@@ -3258,10 +3261,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,7 +3402,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -3408,6 +3411,20 @@
         <v>106</v>
       </c>
       <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3420,8 +3437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3525,11 +3542,14 @@
       <c r="B5" s="14">
         <v>5</v>
       </c>
+      <c r="C5" s="14">
+        <v>4</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
+      <c r="F5" s="27" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3579,7 +3599,7 @@
       </c>
       <c r="C9" s="14">
         <f>SUM(C2:C8)</f>
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -3619,7 +3639,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
PlayerStats affect the stamina and mana cost of items, Store Scene Works, Player can level up
PlayerStats are worked into items now to affect the mana or stamina cost
of an item.
The Player can level up now when they gain enough experience allowing
them to increase their stats

The Store scene works correctly, allowing the player to buy and sell
items.
Updated Clerk to allow items to be added to clerk's inventory

Fixed issue with coinbag that would prevent player from selecting
anything else

Added sound effects to Inventory and Store

InventorySlot updated to support buying, selling, or equipping item

Renamed UI folder in Sounds folder to UI_And_SoundEffects

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="9" r:id="rId2"/>
     <sheet name="BackLog" sheetId="8" r:id="rId3"/>
-    <sheet name="Tasks 03-18 to 03-25" sheetId="11" r:id="rId4"/>
-    <sheet name="Tasks 03-11 to 03-18" sheetId="10" r:id="rId5"/>
-    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId6"/>
-    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId7"/>
-    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId8"/>
-    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId9"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId10"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId11"/>
+    <sheet name="Tasks 03-25 to 04-01" sheetId="12" r:id="rId4"/>
+    <sheet name="Tasks 03-18 to 03-25" sheetId="11" r:id="rId5"/>
+    <sheet name="Tasks 03-11 to 03-18" sheetId="10" r:id="rId6"/>
+    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId7"/>
+    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId8"/>
+    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId9"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId10"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId11"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="291">
   <si>
     <t>Feature</t>
   </si>
@@ -684,9 +685,6 @@
     <t>Load and Save Player stats and inventory</t>
   </si>
   <si>
-    <t>Will be able to re use a lot of the inventory</t>
-  </si>
-  <si>
     <t>Player stats being taken into effect</t>
   </si>
   <si>
@@ -714,9 +712,6 @@
     <t>Have FlyingEnemy fly</t>
   </si>
   <si>
-    <t>Have Inventory Serialized before Deserialization</t>
-  </si>
-  <si>
     <t>Create Temporary Coin holding</t>
   </si>
   <si>
@@ -753,9 +748,6 @@
     <t>In order to not collect coins if the Player losses the level</t>
   </si>
   <si>
-    <t>This way the json file can be altered without having to go into the file and change things manually</t>
-  </si>
-  <si>
     <t>Time Estimate (in hours)</t>
   </si>
   <si>
@@ -856,13 +848,73 @@
   </si>
   <si>
     <t>Add Enemy Burning effect</t>
+  </si>
+  <si>
+    <t>Fix Taps stopping when a coin is collected</t>
+  </si>
+  <si>
+    <t>When the player holds onto a coin icon and drags it to the coinbag without letting go</t>
+  </si>
+  <si>
+    <t>Icons cut to the right when thrown</t>
+  </si>
+  <si>
+    <t>PlayerStats being taken into effect</t>
+  </si>
+  <si>
+    <t>Fix Button not switching between Buy and Sell mode</t>
+  </si>
+  <si>
+    <t>Need to dynamically set the button listener</t>
+  </si>
+  <si>
+    <t>Sold Items are added to the clerks inventory</t>
+  </si>
+  <si>
+    <t>~100%</t>
+  </si>
+  <si>
+    <t>~0</t>
+  </si>
+  <si>
+    <t>Save LeveledUp stat in PlayerStats to store if the player has leveled up</t>
+  </si>
+  <si>
+    <t>In case player exits game before leveling up their character</t>
+  </si>
+  <si>
+    <t>InProgress</t>
+  </si>
+  <si>
+    <t>Add Sound Effects for Enemies</t>
+  </si>
+  <si>
+    <t>Add more sound effects</t>
+  </si>
+  <si>
+    <t>Fix issue</t>
+  </si>
+  <si>
+    <t>Make any necessary adjustments</t>
+  </si>
+  <si>
+    <t>Add Particle effect to Lightning Magic</t>
+  </si>
+  <si>
+    <t>Sound for attack, die, and maybe move</t>
+  </si>
+  <si>
+    <t>Weapon always appears under actionarea</t>
+  </si>
+  <si>
+    <t>Enemy death is delayed if continually attacking enemy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -915,8 +967,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -938,6 +996,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1003,7 +1067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1086,6 +1150,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1374,7 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2408,6 +2475,360 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="14">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="14">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="14">
+        <v>3</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>-2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="14">
+        <v>4</v>
+      </c>
+      <c r="C10" s="14">
+        <v>4</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2.25</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="14">
+        <v>4</v>
+      </c>
+      <c r="C15" s="14">
+        <v>3</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="14">
+        <f>SUM(B2:B15)</f>
+        <v>30.5</v>
+      </c>
+      <c r="C17" s="14">
+        <f>SUM(C2:C16)</f>
+        <v>12.25</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -2712,7 +3133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
@@ -3063,10 +3484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3077,37 +3498,40 @@
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C2" s="36">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="D2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C3" s="36">
         <v>0</v>
@@ -3116,9 +3540,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C4" s="36">
         <v>0.1</v>
@@ -3127,12 +3551,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C5" s="36">
         <v>0.9</v>
@@ -3141,68 +3565,74 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>266</v>
       </c>
       <c r="C6" s="36">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="D6" s="14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>215</v>
       </c>
       <c r="B7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="D8" t="s">
+        <v>279</v>
+      </c>
+      <c r="E8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" t="s">
         <v>232</v>
       </c>
-      <c r="C7" s="36">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B8" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B9" t="s">
-        <v>234</v>
-      </c>
       <c r="C9" s="36">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C10" s="36">
         <v>0</v>
@@ -3211,12 +3641,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C11" s="36">
         <v>0.25</v>
@@ -3225,12 +3655,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C12" s="36">
         <v>0</v>
@@ -3239,12 +3669,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B13" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C13" s="36">
         <v>0.8</v>
@@ -3261,10 +3691,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,7 +3798,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>289</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3379,13 +3809,10 @@
       <c r="F6" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G6" t="s">
-        <v>239</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>246</v>
+        <v>290</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -3394,37 +3821,6 @@
         <v>106</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>272</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="26" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3435,10 +3831,280 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:T13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="14">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+    </row>
+    <row r="4" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+    </row>
+    <row r="5" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" s="14">
+        <v>5</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B9" s="14">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>21</v>
+      </c>
+      <c r="C11" s="14">
+        <f>SUM(C2:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>21</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3452,7 +4118,7 @@
     <col min="7" max="7" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3475,26 +4141,28 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B2" s="14">
         <v>2</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="14">
+        <v>3</v>
+      </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
+      <c r="F2" s="39" t="s">
+        <v>282</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>200</v>
       </c>
@@ -3504,7 +4172,9 @@
       <c r="C3" s="14">
         <v>1</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="14">
+        <v>-1</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
@@ -3512,12 +4182,12 @@
         <v>123</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3525,6 +4195,9 @@
       <c r="C4">
         <v>0.5</v>
       </c>
+      <c r="D4">
+        <v>-0.5</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
@@ -3532,109 +4205,257 @@
         <v>123</v>
       </c>
       <c r="G4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B5" s="14">
         <v>5</v>
       </c>
       <c r="C5" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B6" s="14">
         <v>3</v>
       </c>
+      <c r="C6" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>-0.5</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B7" s="14">
         <v>8</v>
       </c>
+      <c r="C7" s="14">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14">
+        <v>-4</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="29">
+        <v>1</v>
+      </c>
+      <c r="C8" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="29">
+        <v>-0.5</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="G9" s="35"/>
+    </row>
+    <row r="10" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1</v>
+      </c>
+      <c r="C10" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="29">
+        <v>-0.5</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="B11" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="C11" s="29">
+        <v>1</v>
+      </c>
+      <c r="D11" s="29">
+        <v>-0.5</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="35"/>
+    </row>
+    <row r="12" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" s="29">
+        <v>1</v>
+      </c>
+      <c r="C12" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="29">
+        <v>-0.5</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="B13" s="29">
+        <v>4</v>
+      </c>
+      <c r="C13" s="29">
+        <v>2</v>
+      </c>
+      <c r="D13" s="29">
+        <v>-2</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B15" s="14">
         <f>SUM(B2:B7)</f>
         <v>21</v>
       </c>
-      <c r="C9" s="14">
-        <f>SUM(C2:C8)</f>
-        <v>5.5</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="C15" s="14">
+        <f>SUM(C2:C14)</f>
+        <v>20.5</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="14">
-        <f>SUM(B2:B7)</f>
-        <v>21</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="B16" s="14">
+        <f>SUM(B2:B13)</f>
+        <v>30.5</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
@@ -3699,7 +4520,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B3" s="14">
         <v>1.5</v>
@@ -3739,14 +4560,14 @@
         <v>123</v>
       </c>
       <c r="G4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B5" s="14">
         <v>1</v>
@@ -3764,12 +4585,12 @@
         <v>123</v>
       </c>
       <c r="G5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B6" s="14">
         <v>2</v>
@@ -3787,12 +4608,12 @@
         <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B7" s="14">
         <v>3</v>
@@ -3812,7 +4633,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>
@@ -3832,7 +4653,7 @@
     </row>
     <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B9" s="14">
         <v>2</v>
@@ -3852,7 +4673,7 @@
     </row>
     <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B10" s="14">
         <v>2</v>
@@ -3872,7 +4693,7 @@
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B11" s="14">
         <v>2</v>
@@ -3890,12 +4711,12 @@
         <v>123</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B12" s="14">
         <v>2</v>
@@ -3915,7 +4736,7 @@
     </row>
     <row r="13" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B13" s="29">
         <v>2</v>
@@ -3933,12 +4754,12 @@
         <v>123</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B14" s="29">
         <v>0.5</v>
@@ -3958,7 +4779,7 @@
     </row>
     <row r="15" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B15" s="29">
         <v>2</v>
@@ -3978,7 +4799,7 @@
     </row>
     <row r="16" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B16" s="29">
         <v>2</v>
@@ -3996,7 +4817,7 @@
         <v>123</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -4168,7 +4989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
@@ -4251,7 +5072,7 @@
     </row>
     <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B4" s="14">
         <v>6</v>
@@ -4299,7 +5120,7 @@
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
@@ -4393,7 +5214,7 @@
     </row>
     <row r="12" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B12" s="29">
         <v>0.5</v>
@@ -4409,12 +5230,12 @@
         <v>123</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B13" s="29">
         <v>0.5</v>
@@ -4566,7 +5387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
@@ -5003,7 +5824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
@@ -5451,358 +6272,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="14">
-        <v>3</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="C3" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="14">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="14">
-        <v>-0.5</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" s="14">
-        <v>2</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6" s="14">
-        <v>4</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="14">
-        <v>3</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="14">
-        <v>2</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" s="14">
-        <v>3</v>
-      </c>
-      <c r="C9" s="14">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14">
-        <v>-2</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10" s="14">
-        <v>4</v>
-      </c>
-      <c r="C10" s="14">
-        <v>4</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="B11" s="14">
-        <v>2</v>
-      </c>
-      <c r="C11" s="14">
-        <v>2.25</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="B12" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="C12" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="B14" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="C14" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" s="14">
-        <v>4</v>
-      </c>
-      <c r="C15" s="14">
-        <v>3</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="14">
-        <f>SUM(B2:B15)</f>
-        <v>30.5</v>
-      </c>
-      <c r="C17" s="14">
-        <f>SUM(C2:C16)</f>
-        <v>12.25</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L23" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L24" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L25" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
About 33 sound effects added for all of the enemies
Updated Enemy class to support sound effects and Low Health state

Updated FlyingEnemy, RangedEnemy, SpiderBoss, classes to support sound
effects

Added Equip Magic Sound effect to Inventory

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -15,15 +15,16 @@
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="9" r:id="rId2"/>
     <sheet name="BackLog" sheetId="8" r:id="rId3"/>
-    <sheet name="Tasks 03-25 to 04-01" sheetId="12" r:id="rId4"/>
-    <sheet name="Tasks 03-18 to 03-25" sheetId="11" r:id="rId5"/>
-    <sheet name="Tasks 03-11 to 03-18" sheetId="10" r:id="rId6"/>
-    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId7"/>
-    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId8"/>
-    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId9"/>
-    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId10"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId11"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId12"/>
+    <sheet name="Tasks 04-01 to 04-08" sheetId="13" r:id="rId4"/>
+    <sheet name="Tasks 03-25 to 04-01" sheetId="12" r:id="rId5"/>
+    <sheet name="Tasks 03-18 to 03-25" sheetId="11" r:id="rId6"/>
+    <sheet name="Tasks 03-11 to 03-18" sheetId="10" r:id="rId7"/>
+    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId8"/>
+    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId9"/>
+    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId10"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId11"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId12"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="295">
   <si>
     <t>Feature</t>
   </si>
@@ -895,19 +896,31 @@
     <t>Fix issue</t>
   </si>
   <si>
-    <t>Make any necessary adjustments</t>
-  </si>
-  <si>
     <t>Add Particle effect to Lightning Magic</t>
   </si>
   <si>
-    <t>Sound for attack, die, and maybe move</t>
-  </si>
-  <si>
     <t>Weapon always appears under actionarea</t>
   </si>
   <si>
     <t>Enemy death is delayed if continually attacking enemy</t>
+  </si>
+  <si>
+    <t>Replace Luck with Wisdom</t>
+  </si>
+  <si>
+    <t>Sound for attack, die, hit and stand/move</t>
+  </si>
+  <si>
+    <t>Push Perspective back</t>
+  </si>
+  <si>
+    <t>Deal with multiple enemies</t>
+  </si>
+  <si>
+    <t>Display hit points when attacking</t>
+  </si>
+  <si>
+    <t>Sound Effects for the Player</t>
   </si>
 </sst>
 </file>
@@ -2476,6 +2489,456 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="C2" s="14">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="14">
+        <v>4</v>
+      </c>
+      <c r="C5" s="14">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="14">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>-1.5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="14">
+        <v>2</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>19.5</v>
+      </c>
+      <c r="C13" s="14">
+        <f>SUM(C2:C12)</f>
+        <v>12.5</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2828,7 +3291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -3133,7 +3596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
@@ -3798,7 +4261,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3812,7 +4275,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -3831,10 +4294,257 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8" s="14">
+        <v>3</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="14">
+        <v>4</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>25</v>
+      </c>
+      <c r="C13" s="14">
+        <f>SUM(C2:C12)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>25</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="39" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3878,13 +4588,15 @@
       <c r="B2" s="14">
         <v>2</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="14">
+        <v>0.5</v>
+      </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>284</v>
@@ -3938,7 +4650,7 @@
         <v>121</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -3961,16 +4673,18 @@
       <c r="B5" s="14">
         <v>5</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="14">
+        <v>8.5</v>
+      </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -4033,7 +4747,7 @@
     </row>
     <row r="9" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B9" s="14">
         <v>3</v>
@@ -4064,7 +4778,7 @@
       </c>
       <c r="C11" s="14">
         <f>SUM(C2:C10)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -4094,17 +4808,27 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="39" t="s">
+        <v>282</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4455,7 +5179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
@@ -4989,7 +5713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
@@ -5387,7 +6111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
@@ -5822,454 +6546,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="C2" s="14">
-        <v>2</v>
-      </c>
-      <c r="D2" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-    </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="C3" s="14">
-        <v>2</v>
-      </c>
-      <c r="D3" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
-        <v>1</v>
-      </c>
-      <c r="D4" s="14">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="14">
-        <v>4</v>
-      </c>
-      <c r="C5" s="14">
-        <v>2</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="14">
-        <v>3</v>
-      </c>
-      <c r="C6" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D6" s="14">
-        <v>-1.5</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-    </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="B7" s="14">
-        <v>2</v>
-      </c>
-      <c r="C7" s="14">
-        <v>2</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="14">
-        <v>2</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" s="14">
-        <v>1</v>
-      </c>
-      <c r="C9" s="14">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="14">
-        <v>2</v>
-      </c>
-      <c r="C10" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>19.5</v>
-      </c>
-      <c r="C13" s="14">
-        <f>SUM(C2:C12)</f>
-        <v>12.5</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more sound effects, Added new particle effects, improved current particles effets.
Added Sound Effects for coin collection, potion drinking, fire effect,
ice effect, lightning, and ranged icon

Added particle effects for being frozen and catching on fire and using
lightning

Improved particle effects for frost blast and fire blast

Changed Luck stat to Wisdom stat

EnemySpawner now properly ends the level when all enemies have been
killed (preparation for next week)

Updated Player class to support wisdom stat

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="300">
   <si>
     <t>Feature</t>
   </si>
@@ -701,9 +701,6 @@
     <t>What is left to do?</t>
   </si>
   <si>
-    <t>Weaknesses implemented into enemies</t>
-  </si>
-  <si>
     <t>Player leveling up(player being able to control their stats)</t>
   </si>
   <si>
@@ -740,9 +737,6 @@
     <t>Move, attack, die</t>
   </si>
   <si>
-    <t>Magic and Weapons being more or less effective against enemies</t>
-  </si>
-  <si>
     <t>Combat System</t>
   </si>
   <si>
@@ -842,9 +836,6 @@
     <t>Polish/fix an potential bugs</t>
   </si>
   <si>
-    <t>Magic, Enemy sounds, Weapon sounds</t>
-  </si>
-  <si>
     <t>Add Enemy Froze Effect</t>
   </si>
   <si>
@@ -890,9 +881,6 @@
     <t>Add Sound Effects for Enemies</t>
   </si>
   <si>
-    <t>Add more sound effects</t>
-  </si>
-  <si>
     <t>Fix issue</t>
   </si>
   <si>
@@ -921,6 +909,33 @@
   </si>
   <si>
     <t>Sound Effects for the Player</t>
+  </si>
+  <si>
+    <t>with sound</t>
+  </si>
+  <si>
+    <t>Fix enemy shrinking when slowed down</t>
+  </si>
+  <si>
+    <t>Add more bosses</t>
+  </si>
+  <si>
+    <t>Improved Fire and Frost particle effects</t>
+  </si>
+  <si>
+    <t>Added better particle effects</t>
+  </si>
+  <si>
+    <t>Add magic equip sound effect, rangedIconSound effect, frost blast sound effect, fireblast sound effect, potion drank sound effect</t>
+  </si>
+  <si>
+    <t>Add Enemy Electrocuted Sound Effect</t>
+  </si>
+  <si>
+    <t>Enemy sounds, Weapon sounds</t>
+  </si>
+  <si>
+    <t>Adjust enemy speeds to increase difficulty</t>
   </si>
 </sst>
 </file>
@@ -3947,10 +3962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3969,10 +3984,10 @@
         <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E1" t="s">
         <v>104</v>
@@ -3983,18 +3998,18 @@
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>298</v>
       </c>
       <c r="C2" s="36">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C3" s="36">
         <v>0</v>
@@ -4005,13 +4020,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="36">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4019,7 +4034,7 @@
         <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C5" s="36">
         <v>0.9</v>
@@ -4033,7 +4048,7 @@
         <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" s="36">
         <v>0.9</v>
@@ -4047,13 +4062,13 @@
         <v>215</v>
       </c>
       <c r="B7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>123</v>
@@ -4061,16 +4076,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E8" t="s">
         <v>123</v>
@@ -4081,13 +4096,16 @@
         <v>216</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C9" s="36">
-        <v>0.8</v>
+        <v>231</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>275</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4095,7 +4113,7 @@
         <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C10" s="36">
         <v>0</v>
@@ -4109,40 +4127,26 @@
         <v>217</v>
       </c>
       <c r="B11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C11" s="36">
         <v>0.25</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>265</v>
       </c>
       <c r="C12" s="36">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>235</v>
-      </c>
-      <c r="B13" t="s">
-        <v>267</v>
-      </c>
-      <c r="C13" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="D13">
         <v>6</v>
       </c>
     </row>
@@ -4154,10 +4158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E10" sqref="E10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4261,7 +4265,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -4275,7 +4279,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -4284,6 +4288,34 @@
         <v>106</v>
       </c>
       <c r="F7" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B8" s="14">
+        <v>4</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4294,15 +4326,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -4310,7 +4342,7 @@
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -4332,7 +4364,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -4348,10 +4380,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>274</v>
+        <v>241</v>
       </c>
       <c r="B3" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -4362,15 +4394,13 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>243</v>
+        <v>287</v>
       </c>
       <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+        <v>3</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
@@ -4378,15 +4408,13 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="B5" s="14">
-        <v>3</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+        <v>1</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
@@ -4394,15 +4422,13 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="B6" s="14">
-        <v>4</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+        <v>1</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
@@ -4410,15 +4436,13 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="B7" s="14">
-        <v>3</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+        <v>10</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
@@ -4426,11 +4450,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="B8" s="14">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
       <c r="E8" s="14" t="s">
@@ -4440,98 +4464,56 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="B9" s="14">
-        <v>2</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="26" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="14">
+        <f>SUM(B2:B8)</f>
+        <v>21</v>
+      </c>
+      <c r="C10" s="14">
+        <f>SUM(C2:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="14">
+        <f>SUM(B2:B8)</f>
+        <v>21</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="B10" s="14">
-        <v>2</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="B11" s="14">
-        <v>4</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>25</v>
-      </c>
-      <c r="C13" s="14">
-        <f>SUM(C2:C12)</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-    </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B14" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>25</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I15" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I16" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="39" t="s">
-        <v>282</v>
+      <c r="I14" s="39" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -4541,10 +4523,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4583,13 +4565,13 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B2" s="14">
         <v>2</v>
       </c>
       <c r="C2" s="14">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
@@ -4599,12 +4581,12 @@
         <v>123</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
@@ -4618,7 +4600,7 @@
         <v>121</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -4636,21 +4618,23 @@
     </row>
     <row r="4" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="14">
+        <v>0.5</v>
+      </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -4668,7 +4652,7 @@
     </row>
     <row r="5" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B5" s="14">
         <v>5</v>
@@ -4684,7 +4668,7 @@
         <v>123</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -4702,7 +4686,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -4714,85 +4698,110 @@
         <v>121</v>
       </c>
       <c r="G6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
+      <c r="C8">
+        <v>2.5</v>
+      </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B9" s="14">
         <v>3</v>
       </c>
+      <c r="C9" s="14">
+        <v>2</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" s="14">
-        <f>SUM(B2:B9)</f>
-        <v>21</v>
-      </c>
-      <c r="C11" s="14">
-        <f>SUM(C2:C10)</f>
-        <v>9</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="38">
+        <v>1</v>
+      </c>
+      <c r="C10" s="38">
+        <v>1</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" s="38">
+        <v>1</v>
+      </c>
+      <c r="C11" s="38">
+        <v>1</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" s="14">
-        <f>SUM(B2:B9)</f>
-        <v>21</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -4800,22 +4809,53 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>21</v>
+      </c>
+      <c r="C13" s="14">
+        <f>SUM(C2:C12)</f>
+        <v>20.5</v>
+      </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="39" t="s">
-        <v>282</v>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>23</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="39" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -4867,7 +4907,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B2" s="14">
         <v>2</v>
@@ -4880,10 +4920,10 @@
         <v>106</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -4906,12 +4946,12 @@
         <v>123</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4929,12 +4969,12 @@
         <v>123</v>
       </c>
       <c r="G4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B5" s="14">
         <v>5</v>
@@ -4951,7 +4991,7 @@
     </row>
     <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B6" s="14">
         <v>3</v>
@@ -4971,7 +5011,7 @@
     </row>
     <row r="7" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B7" s="14">
         <v>8</v>
@@ -4991,7 +5031,7 @@
     </row>
     <row r="8" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B8" s="29">
         <v>1</v>
@@ -5009,12 +5049,12 @@
         <v>123</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B9" s="29">
         <v>1</v>
@@ -5031,7 +5071,7 @@
     </row>
     <row r="10" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B10" s="29">
         <v>1</v>
@@ -5049,12 +5089,12 @@
         <v>123</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B11" s="29">
         <v>1.5</v>
@@ -5075,7 +5115,7 @@
     </row>
     <row r="12" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B12" s="29">
         <v>1</v>
@@ -5093,12 +5133,12 @@
         <v>123</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B13" s="29">
         <v>4</v>
@@ -5113,7 +5153,7 @@
         <v>106</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
@@ -5244,7 +5284,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B3" s="14">
         <v>1.5</v>
@@ -5284,14 +5324,14 @@
         <v>123</v>
       </c>
       <c r="G4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B5" s="14">
         <v>1</v>
@@ -5309,12 +5349,12 @@
         <v>123</v>
       </c>
       <c r="G5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B6" s="14">
         <v>2</v>
@@ -5332,12 +5372,12 @@
         <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B7" s="14">
         <v>3</v>
@@ -5357,7 +5397,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>
@@ -5377,7 +5417,7 @@
     </row>
     <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B9" s="14">
         <v>2</v>
@@ -5397,7 +5437,7 @@
     </row>
     <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B10" s="14">
         <v>2</v>
@@ -5417,7 +5457,7 @@
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B11" s="14">
         <v>2</v>
@@ -5435,12 +5475,12 @@
         <v>123</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B12" s="14">
         <v>2</v>
@@ -5460,7 +5500,7 @@
     </row>
     <row r="13" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B13" s="29">
         <v>2</v>
@@ -5478,12 +5518,12 @@
         <v>123</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B14" s="29">
         <v>0.5</v>
@@ -5503,7 +5543,7 @@
     </row>
     <row r="15" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B15" s="29">
         <v>2</v>
@@ -5523,7 +5563,7 @@
     </row>
     <row r="16" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B16" s="29">
         <v>2</v>
@@ -5541,7 +5581,7 @@
         <v>123</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -5844,7 +5884,7 @@
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
@@ -5954,12 +5994,12 @@
         <v>123</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B13" s="29">
         <v>0.5</v>

</xml_diff>

<commit_message>
Added layers to enemy playing field, added multiple enemies to levels
Added layers to level to allow multiple enemies at different layers in
the level

Added multiple enemies to each level

altered enemy stats to increase difficulty

Updated enemy class to improve movement and scaling

added Damage text that appears above an enemy when they are damaged

Added more sound effects to character scene

Decreased cost of potions and repair hammers

Fixed Icon turning in the wrong direction issue

Players can only play levels they have unlocked

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="6630" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="9" r:id="rId2"/>
     <sheet name="BackLog" sheetId="8" r:id="rId3"/>
-    <sheet name="Tasks 04-01 to 04-08" sheetId="13" r:id="rId4"/>
-    <sheet name="Tasks 03-25 to 04-01" sheetId="12" r:id="rId5"/>
-    <sheet name="Tasks 03-18 to 03-25" sheetId="11" r:id="rId6"/>
-    <sheet name="Tasks 03-11 to 03-18" sheetId="10" r:id="rId7"/>
-    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId8"/>
-    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId9"/>
-    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId10"/>
-    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId11"/>
-    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId12"/>
-    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId13"/>
+    <sheet name="Tasks 04-08 to 04-15" sheetId="14" r:id="rId4"/>
+    <sheet name="Tasks 04-01 to 04-08" sheetId="13" r:id="rId5"/>
+    <sheet name="Tasks 03-25 to 04-01" sheetId="12" r:id="rId6"/>
+    <sheet name="Tasks 03-18 to 03-25" sheetId="11" r:id="rId7"/>
+    <sheet name="Tasks 03-11 to 03-18" sheetId="10" r:id="rId8"/>
+    <sheet name="Tasks 03-04 to 03-11" sheetId="7" r:id="rId9"/>
+    <sheet name="Tasks 02-25 to 03-04" sheetId="6" r:id="rId10"/>
+    <sheet name="Tasks 02-18 to 02-25" sheetId="5" r:id="rId11"/>
+    <sheet name="Tasks 02-11 to 02-18" sheetId="4" r:id="rId12"/>
+    <sheet name="Tasks 02-04 to 02-11" sheetId="3" r:id="rId13"/>
+    <sheet name="Tasks 01-28 to 02-04" sheetId="2" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="314">
   <si>
     <t>Feature</t>
   </si>
@@ -899,9 +900,6 @@
     <t>Sound for attack, die, hit and stand/move</t>
   </si>
   <si>
-    <t>Push Perspective back</t>
-  </si>
-  <si>
     <t>Deal with multiple enemies</t>
   </si>
   <si>
@@ -935,7 +933,52 @@
     <t>Enemy sounds, Weapon sounds</t>
   </si>
   <si>
-    <t>Adjust enemy speeds to increase difficulty</t>
+    <t>Play Testing and Game Balancing</t>
+  </si>
+  <si>
+    <t>Push Perspective back/Add Layers to enemy positions</t>
+  </si>
+  <si>
+    <t>Add visual indications that the player has been hit</t>
+  </si>
+  <si>
+    <t>Adjust enemy attack times, health, and speeds. Adjust Player stats, speed up icons</t>
+  </si>
+  <si>
+    <t>Unlock levels as you progress</t>
+  </si>
+  <si>
+    <t>Ice rendering behind enemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice or fire not moving with enemy </t>
+  </si>
+  <si>
+    <t>Icons getting stuck when spider does special attack</t>
+  </si>
+  <si>
+    <t>Make more weapons and shields</t>
+  </si>
+  <si>
+    <t>Improve colliders on enemies</t>
+  </si>
+  <si>
+    <t>Add back button to scenes</t>
+  </si>
+  <si>
+    <t>Blocking with shield, player being hit, player dies, etc</t>
+  </si>
+  <si>
+    <t>When hit twice with fire or ice</t>
+  </si>
+  <si>
+    <t>Fix damage done by damageovertime</t>
+  </si>
+  <si>
+    <t>Look into why Shield is so slow to be selected</t>
+  </si>
+  <si>
+    <t>Come up with new algorithm for experience</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2503,6 +2546,443 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L21:L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="25">
+        <v>3</v>
+      </c>
+      <c r="C2" s="25">
+        <v>1</v>
+      </c>
+      <c r="D2" s="25">
+        <v>-2</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="14">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="14">
+        <v>-2.5</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="14">
+        <f>SUM(B2:B12)</f>
+        <v>20</v>
+      </c>
+      <c r="C14" s="14">
+        <f>SUM(C2:C13)</f>
+        <v>12.5</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
@@ -2952,7 +3432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -3306,7 +3786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -3611,7 +4091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
@@ -3965,7 +4445,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3998,7 +4478,7 @@
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C2" s="36">
         <v>0.75</v>
@@ -4158,10 +4638,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:F10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4265,10 +4745,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
@@ -4279,10 +4759,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>284</v>
+        <v>307</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
@@ -4291,12 +4771,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="B8" s="14">
-        <v>4</v>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
@@ -4307,15 +4787,43 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>313</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="26" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4326,23 +4834,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -4361,16 +4868,17 @@
       <c r="F1" s="25" t="s">
         <v>104</v>
       </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="B2" s="14">
-        <v>1</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
@@ -4379,14 +4887,12 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="B3" s="14">
-        <v>2</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="A3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
@@ -4396,10 +4902,10 @@
     </row>
     <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B4" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
@@ -4407,13 +4913,16 @@
       <c r="F4" s="26" t="s">
         <v>121</v>
       </c>
+      <c r="G4" s="14" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B5" s="14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
@@ -4422,11 +4931,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="B6" s="14">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
       <c r="E6" s="14" t="s">
@@ -4436,12 +4945,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="B7" s="14">
-        <v>10</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
@@ -4449,13 +4958,16 @@
       <c r="F7" s="26" t="s">
         <v>121</v>
       </c>
+      <c r="G7" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
@@ -4465,54 +4977,101 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="A9" t="s">
+        <v>306</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B10" s="14">
-        <f>SUM(B2:B8)</f>
-        <v>21</v>
-      </c>
-      <c r="C10" s="14">
-        <f>SUM(C2:C9)</f>
-        <v>0</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>208</v>
+      <c r="A11" s="14" t="s">
+        <v>207</v>
       </c>
       <c r="B11" s="14">
-        <f>SUM(B2:B8)</f>
+        <f>SUM(B2:B9)</f>
         <v>21</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="14">
+        <f>SUM(C2:C10)</f>
+        <v>0</v>
+      </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I12" s="28" t="s">
-        <v>123</v>
-      </c>
+      <c r="A12" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>21</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I13" s="26" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I14" s="39" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="39" t="s">
         <v>279</v>
       </c>
     </row>
@@ -4522,6 +5081,254 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14">
+        <v>-2</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="14">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>8.5</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="G7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2.5</v>
+      </c>
+      <c r="D8">
+        <v>-0.5</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="38">
+        <v>1</v>
+      </c>
+      <c r="C9" s="38">
+        <v>1</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="14">
+        <f>SUM(B2:B8)</f>
+        <v>21</v>
+      </c>
+      <c r="C11" s="14">
+        <f>SUM(C2:C10)</f>
+        <v>19</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="14">
+        <f>SUM(B2:B9)</f>
+        <v>22</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T25"/>
   <sheetViews>
@@ -4581,7 +5388,7 @@
         <v>123</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4718,7 +5525,7 @@
         <v>123</v>
       </c>
       <c r="G7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -4738,7 +5545,7 @@
         <v>123</v>
       </c>
       <c r="G8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4758,32 +5565,32 @@
         <v>123</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" s="38">
+        <v>1</v>
+      </c>
+      <c r="C10" s="38">
+        <v>1</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="35" t="s">
         <v>294</v>
-      </c>
-      <c r="B10" s="38">
-        <v>1</v>
-      </c>
-      <c r="C10" s="38">
-        <v>1</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B11" s="38">
         <v>1</v>
@@ -4863,7 +5670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
@@ -5219,7 +6026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
@@ -5753,7 +6560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
@@ -6149,441 +6956,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L21:L22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="25">
-        <v>3</v>
-      </c>
-      <c r="C2" s="25">
-        <v>1</v>
-      </c>
-      <c r="D2" s="25">
-        <v>-2</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="14">
-        <v>2</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
-        <v>2</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B5" s="14">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14">
-        <v>1</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="B7" s="14">
-        <v>4</v>
-      </c>
-      <c r="C7" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D7" s="14">
-        <v>-2.5</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="14">
-        <v>2</v>
-      </c>
-      <c r="C8" s="14">
-        <v>2</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="C9" s="14">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14">
-        <v>-0.5</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="C10" s="14">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14">
-        <v>-0.5</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="B12" s="14">
-        <v>2</v>
-      </c>
-      <c r="C12" s="14">
-        <v>2</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="14">
-        <f>SUM(B2:B12)</f>
-        <v>20</v>
-      </c>
-      <c r="C14" s="14">
-        <f>SUM(C2:C13)</f>
-        <v>12.5</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added back buttons and quit button, Added bow graphic when using arrows
Visual added to indicate what levels are locked and what levels are
unlocked

Added back and quit buttons

Added bow graphic for arrow use

Added trails to coin icons, weapons, and ranged icons

Changed all enemies to use polygon colliders
Fixed damageovertime for enemy
Fixed ice rendering behind enemy

Added DamageText prefab to spawn in text during level when needed (used
in numerous spots)

Updated End Game Menu text to display some level stats

Decreased fingerRadius on inventoryslots to reduce accidental taps

Added app icon to game

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityGames\RPGHeroPrototype\TechnicalDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\UnityGames\RPGHeroPrototype\TechnicalDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="9" r:id="rId2"/>
     <sheet name="BackLog" sheetId="8" r:id="rId3"/>
-    <sheet name="Tasks 04-08 to 04-15" sheetId="14" r:id="rId4"/>
+    <sheet name="Tasks 04-08 to 04-21" sheetId="14" r:id="rId4"/>
     <sheet name="Tasks 04-01 to 04-08" sheetId="13" r:id="rId5"/>
     <sheet name="Tasks 03-25 to 04-01" sheetId="12" r:id="rId6"/>
     <sheet name="Tasks 03-18 to 03-25" sheetId="11" r:id="rId7"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="331">
   <si>
     <t>Feature</t>
   </si>
@@ -963,9 +963,6 @@
     <t>Blocking with shield, player being hit, player dies, etc</t>
   </si>
   <si>
-    <t>When hit twice with fire or ice</t>
-  </si>
-  <si>
     <t>Fix damage done by damageovertime</t>
   </si>
   <si>
@@ -988,6 +985,51 @@
   </si>
   <si>
     <t>Improve visuals of attacking enemy, like health reducing make it wiggle/ show life</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Working on DamageText</t>
+  </si>
+  <si>
+    <t>Added trails to weapon, arrows, eagle, and coins</t>
+  </si>
+  <si>
+    <t>Show if level is unlocked or locked</t>
+  </si>
+  <si>
+    <t>Weapon now appears above</t>
+  </si>
+  <si>
+    <t>Seemed to no longer occur</t>
+  </si>
+  <si>
+    <t>ice now renders in front always</t>
+  </si>
+  <si>
+    <t>ice and fire continually move now</t>
+  </si>
+  <si>
+    <t>All enemies now use polygon colliders</t>
+  </si>
+  <si>
+    <t>Correct amount of damage is now being done</t>
+  </si>
+  <si>
+    <t>Back buttons are in place now and Improved character scene placement of plus minus and rearranged the inventory and store scenes</t>
+  </si>
+  <si>
+    <t>Added Icon image, increased button sizes</t>
+  </si>
+  <si>
+    <t>Improved end game text</t>
+  </si>
+  <si>
+    <t>Added bow Graphic to rangedicons</t>
+  </si>
+  <si>
+    <t>Have all icons rotate in the direction they are thrown</t>
   </si>
 </sst>
 </file>
@@ -1525,15 +1567,15 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" customWidth="1"/>
-    <col min="6" max="6" width="255.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="255.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1553,7 +1595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1563,7 +1605,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>7</v>
       </c>
@@ -1583,7 +1625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="13"/>
       <c r="C4" s="23"/>
@@ -1591,7 +1633,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
@@ -1609,7 +1651,7 @@
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="13" t="s">
         <v>99</v>
@@ -1625,7 +1667,7 @@
       </c>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1635,7 +1677,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
@@ -1655,7 +1697,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1663,7 +1705,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -1683,7 +1725,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="10"/>
       <c r="C11" s="17"/>
@@ -1691,7 +1733,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1711,7 +1753,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
@@ -1719,7 +1761,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>81</v>
       </c>
@@ -1739,7 +1781,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
         <v>83</v>
@@ -1757,7 +1799,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
         <v>84</v>
@@ -1775,7 +1817,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15" t="s">
         <v>85</v>
@@ -1793,7 +1835,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="10"/>
       <c r="C18" s="17"/>
@@ -1801,7 +1843,7 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -1821,7 +1863,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="9" t="s">
         <v>97</v>
@@ -1839,7 +1881,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
@@ -1849,7 +1891,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1869,7 +1911,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="9" t="s">
         <v>63</v>
@@ -1887,7 +1929,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="9" t="s">
         <v>64</v>
@@ -1905,7 +1947,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1913,7 +1955,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>71</v>
       </c>
@@ -1933,7 +1975,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="9" t="s">
         <v>72</v>
@@ -1951,7 +1993,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="9" t="s">
         <v>90</v>
@@ -1969,7 +2011,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="10"/>
       <c r="C30" s="17"/>
@@ -1977,7 +2019,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>65</v>
       </c>
@@ -1997,7 +2039,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="9" t="s">
         <v>67</v>
@@ -2015,7 +2057,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="9" t="s">
         <v>68</v>
@@ -2033,7 +2075,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="9" t="s">
         <v>70</v>
@@ -2051,7 +2093,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="9" t="s">
         <v>69</v>
@@ -2069,7 +2111,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="10" t="s">
         <v>107</v>
@@ -2087,7 +2129,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -2095,7 +2137,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>109</v>
       </c>
@@ -2107,7 +2149,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>110</v>
@@ -2117,7 +2159,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>112</v>
@@ -2127,7 +2169,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -2135,7 +2177,7 @@
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>113</v>
       </c>
@@ -2145,7 +2187,7 @@
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -2153,7 +2195,7 @@
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
     </row>
-    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>114</v>
       </c>
@@ -2165,7 +2207,7 @@
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
     </row>
-    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>116</v>
@@ -2175,7 +2217,7 @@
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>117</v>
@@ -2185,7 +2227,7 @@
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
     </row>
-    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>118</v>
@@ -2195,7 +2237,7 @@
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -2203,7 +2245,7 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>11</v>
       </c>
@@ -2213,7 +2255,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>13</v>
       </c>
@@ -2233,7 +2275,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="9" t="s">
         <v>41</v>
@@ -2251,7 +2293,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="9" t="s">
         <v>44</v>
@@ -2269,7 +2311,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="9" t="s">
         <v>45</v>
@@ -2287,7 +2329,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="9" t="s">
         <v>46</v>
@@ -2305,7 +2347,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="9" t="s">
         <v>47</v>
@@ -2321,7 +2363,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="10"/>
       <c r="C56" s="17"/>
@@ -2329,7 +2371,7 @@
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>14</v>
       </c>
@@ -2349,7 +2391,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -2357,7 +2399,7 @@
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>15</v>
       </c>
@@ -2377,7 +2419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="14" t="s">
         <v>54</v>
@@ -2395,11 +2437,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
       <c r="B61" s="24"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>16</v>
       </c>
@@ -2409,7 +2451,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>17</v>
       </c>
@@ -2429,7 +2471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="9" t="s">
         <v>19</v>
@@ -2447,7 +2489,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="9" t="s">
         <v>20</v>
@@ -2465,7 +2507,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="9" t="s">
         <v>33</v>
@@ -2483,7 +2525,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="15" t="s">
         <v>31</v>
@@ -2501,7 +2543,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17"/>
       <c r="B68" s="15" t="s">
         <v>32</v>
@@ -2519,7 +2561,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17"/>
       <c r="B69" s="15" t="s">
         <v>34</v>
@@ -2537,7 +2579,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C71" s="14"/>
       <c r="D71" s="20" t="s">
         <v>21</v>
@@ -2562,18 +2604,18 @@
       <selection activeCell="L22" sqref="L21:L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2601,7 +2643,7 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>182</v>
       </c>
@@ -2622,7 +2664,7 @@
       </c>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>175</v>
       </c>
@@ -2646,7 +2688,7 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>177</v>
       </c>
@@ -2666,7 +2708,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>179</v>
       </c>
@@ -2689,7 +2731,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>189</v>
       </c>
@@ -2712,7 +2754,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>186</v>
       </c>
@@ -2732,7 +2774,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>198</v>
       </c>
@@ -2752,7 +2794,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>187</v>
       </c>
@@ -2772,7 +2814,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>188</v>
       </c>
@@ -2792,7 +2834,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>190</v>
       </c>
@@ -2812,7 +2854,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>193</v>
       </c>
@@ -2832,7 +2874,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -2846,7 +2888,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>120</v>
       </c>
@@ -2868,7 +2910,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -2882,7 +2924,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -2896,7 +2938,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -2910,7 +2952,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -2924,7 +2966,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -2938,7 +2980,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -2954,7 +2996,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -2970,7 +3012,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -2999,18 +3041,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.73046875" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3038,7 +3080,7 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>183</v>
       </c>
@@ -3064,7 +3106,7 @@
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>184</v>
       </c>
@@ -3087,7 +3129,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>156</v>
       </c>
@@ -3115,7 +3157,7 @@
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>155</v>
       </c>
@@ -3141,7 +3183,7 @@
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>157</v>
       </c>
@@ -3169,7 +3211,7 @@
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>185</v>
       </c>
@@ -3186,7 +3228,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>175</v>
       </c>
@@ -3210,7 +3252,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>174</v>
       </c>
@@ -3236,7 +3278,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>173</v>
       </c>
@@ -3262,7 +3304,7 @@
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>178</v>
       </c>
@@ -3282,7 +3324,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -3296,7 +3338,7 @@
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>120</v>
       </c>
@@ -3318,7 +3360,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -3332,7 +3374,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -3346,7 +3388,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -3360,7 +3402,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -3374,7 +3416,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -3388,7 +3430,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -3404,7 +3446,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -3420,7 +3462,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -3449,16 +3491,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3482,7 +3524,7 @@
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>154</v>
       </c>
@@ -3500,7 +3542,7 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>152</v>
       </c>
@@ -3522,7 +3564,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>160</v>
       </c>
@@ -3546,7 +3588,7 @@
       </c>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>156</v>
       </c>
@@ -3563,7 +3605,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>155</v>
       </c>
@@ -3577,7 +3619,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>157</v>
       </c>
@@ -3591,7 +3633,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>131</v>
       </c>
@@ -3610,7 +3652,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>159</v>
       </c>
@@ -3630,7 +3672,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>166</v>
       </c>
@@ -3647,7 +3689,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>165</v>
       </c>
@@ -3667,7 +3709,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>163</v>
       </c>
@@ -3687,7 +3729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>164</v>
       </c>
@@ -3707,7 +3749,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>167</v>
       </c>
@@ -3727,7 +3769,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>172</v>
       </c>
@@ -3747,7 +3789,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -3757,7 +3799,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>120</v>
       </c>
@@ -3775,17 +3817,17 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L23" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L24" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L25" s="28" t="s">
         <v>123</v>
       </c>
@@ -3803,16 +3845,16 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.265625" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -3835,7 +3877,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>151</v>
       </c>
@@ -3856,7 +3898,7 @@
       </c>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>142</v>
       </c>
@@ -3877,7 +3919,7 @@
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>143</v>
       </c>
@@ -3900,7 +3942,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>144</v>
       </c>
@@ -3921,7 +3963,7 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>152</v>
       </c>
@@ -3938,7 +3980,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>145</v>
       </c>
@@ -3961,7 +4003,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>148</v>
       </c>
@@ -3984,7 +4026,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>146</v>
       </c>
@@ -4010,7 +4052,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>131</v>
       </c>
@@ -4032,7 +4074,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>150</v>
       </c>
@@ -4052,7 +4094,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>153</v>
       </c>
@@ -4069,7 +4111,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -4078,7 +4120,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>120</v>
       </c>
@@ -4108,19 +4150,19 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.73046875" customWidth="1"/>
-    <col min="3" max="3" width="14.1328125" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.73046875" customWidth="1"/>
-    <col min="13" max="13" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -4143,7 +4185,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -4163,7 +4205,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>125</v>
       </c>
@@ -4186,7 +4228,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -4206,7 +4248,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -4229,7 +4271,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -4249,7 +4291,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -4269,7 +4311,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4292,7 +4334,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -4318,7 +4360,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -4341,7 +4383,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -4367,7 +4409,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -4387,7 +4429,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -4407,7 +4449,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -4430,7 +4472,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -4457,15 +4499,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>220</v>
       </c>
@@ -4482,7 +4524,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -4496,7 +4538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>226</v>
       </c>
@@ -4507,7 +4549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>225</v>
       </c>
@@ -4518,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -4532,7 +4574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -4546,7 +4588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>215</v>
       </c>
@@ -4563,7 +4605,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -4580,7 +4622,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>216</v>
       </c>
@@ -4597,7 +4639,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>205</v>
       </c>
@@ -4611,7 +4653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>217</v>
       </c>
@@ -4625,7 +4667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>233</v>
       </c>
@@ -4653,15 +4695,15 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -4684,7 +4726,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>194</v>
       </c>
@@ -4701,7 +4743,7 @@
       </c>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>195</v>
       </c>
@@ -4718,7 +4760,7 @@
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>196</v>
       </c>
@@ -4735,7 +4777,7 @@
       </c>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>197</v>
       </c>
@@ -4752,9 +4794,9 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4766,9 +4808,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B7">
         <v>1.5</v>
@@ -4780,10 +4822,10 @@
         <v>121</v>
       </c>
       <c r="G7" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>304</v>
       </c>
@@ -4797,7 +4839,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>292</v>
       </c>
@@ -4811,9 +4853,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4832,22 +4874,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -4870,35 +4913,53 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>283</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
       <c r="E2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>284</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>289</v>
       </c>
@@ -4915,38 +4976,53 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>302</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F5" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>316</v>
+      </c>
+      <c r="H5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>303</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>121</v>
+      <c r="F6" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+        <v>316</v>
+      </c>
+      <c r="H6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>300</v>
       </c>
@@ -4960,140 +5036,256 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>305</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F8" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="H8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F9" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" t="s">
+        <v>316</v>
+      </c>
+      <c r="H9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>306</v>
       </c>
       <c r="B10">
         <v>2.5</v>
       </c>
+      <c r="C10">
+        <v>1.5</v>
+      </c>
       <c r="E10" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="C14" s="14">
+        <v>5</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="14" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B21" s="14">
         <f>SUM(B2:B11)</f>
         <v>14.5</v>
       </c>
-      <c r="C14" s="14">
-        <f>SUM(C2:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="31" t="s">
+      <c r="C21" s="14">
+        <f>SUM(C2:C20)</f>
+        <v>15.5</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B22" s="14">
         <f>SUM(B2:B11)</f>
         <v>14.5</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="26" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="39" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="39" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5110,18 +5302,18 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -5141,7 +5333,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>270</v>
       </c>
@@ -5159,7 +5351,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>241</v>
       </c>
@@ -5179,7 +5371,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>299</v>
       </c>
@@ -5199,7 +5391,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>287</v>
       </c>
@@ -5219,7 +5411,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>288</v>
       </c>
@@ -5236,7 +5428,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>298</v>
       </c>
@@ -5253,10 +5445,10 @@
         <v>279</v>
       </c>
       <c r="G7" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>291</v>
       </c>
@@ -5276,7 +5468,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>301</v>
       </c>
@@ -5293,7 +5485,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -5301,7 +5493,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>207</v>
       </c>
@@ -5317,7 +5509,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>208</v>
       </c>
@@ -5330,17 +5522,17 @@
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I13" s="28" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I14" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I15" s="39" t="s">
         <v>279</v>
       </c>
@@ -5358,18 +5550,18 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -5392,7 +5584,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>257</v>
       </c>
@@ -5413,7 +5605,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>270</v>
       </c>
@@ -5445,7 +5637,7 @@
       <c r="S3" s="14"/>
       <c r="T3" s="14"/>
     </row>
-    <row r="4" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>271</v>
       </c>
@@ -5479,7 +5671,7 @@
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
     </row>
-    <row r="5" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>280</v>
       </c>
@@ -5513,7 +5705,7 @@
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>241</v>
       </c>
@@ -5530,7 +5722,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>267</v>
       </c>
@@ -5550,7 +5742,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>266</v>
       </c>
@@ -5570,7 +5762,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>282</v>
       </c>
@@ -5590,7 +5782,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>293</v>
       </c>
@@ -5610,7 +5802,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>296</v>
       </c>
@@ -5628,7 +5820,7 @@
       </c>
       <c r="G11" s="35"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -5637,7 +5829,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>207</v>
       </c>
@@ -5654,7 +5846,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>208</v>
       </c>
@@ -5668,7 +5860,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -5677,12 +5869,12 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G24" s="28" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G25" s="39" t="s">
         <v>279</v>
       </c>
@@ -5700,18 +5892,18 @@
       <selection activeCell="F13" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -5734,7 +5926,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>257</v>
       </c>
@@ -5755,7 +5947,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>200</v>
       </c>
@@ -5778,7 +5970,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -5801,7 +5993,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>238</v>
       </c>
@@ -5818,7 +6010,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>239</v>
       </c>
@@ -5838,7 +6030,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>240</v>
       </c>
@@ -5858,7 +6050,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>268</v>
       </c>
@@ -5881,7 +6073,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>270</v>
       </c>
@@ -5898,7 +6090,7 @@
       </c>
       <c r="G9" s="35"/>
     </row>
-    <row r="10" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>272</v>
       </c>
@@ -5921,7 +6113,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>274</v>
       </c>
@@ -5942,7 +6134,7 @@
       </c>
       <c r="G11" s="35"/>
     </row>
-    <row r="12" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>277</v>
       </c>
@@ -5965,7 +6157,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>271</v>
       </c>
@@ -5993,7 +6185,7 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -6002,7 +6194,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>207</v>
       </c>
@@ -6019,7 +6211,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>208</v>
       </c>
@@ -6033,7 +6225,7 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -6056,17 +6248,17 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -6089,7 +6281,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>201</v>
       </c>
@@ -6111,7 +6303,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>242</v>
       </c>
@@ -6133,7 +6325,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>199</v>
       </c>
@@ -6158,7 +6350,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>243</v>
       </c>
@@ -6181,7 +6373,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>244</v>
       </c>
@@ -6204,7 +6396,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>245</v>
       </c>
@@ -6224,7 +6416,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>246</v>
       </c>
@@ -6244,7 +6436,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>236</v>
       </c>
@@ -6264,7 +6456,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>247</v>
       </c>
@@ -6284,7 +6476,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>256</v>
       </c>
@@ -6307,7 +6499,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>263</v>
       </c>
@@ -6327,7 +6519,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>248</v>
       </c>
@@ -6350,7 +6542,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>249</v>
       </c>
@@ -6370,7 +6562,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>250</v>
       </c>
@@ -6390,7 +6582,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>253</v>
       </c>
@@ -6413,7 +6605,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -6436,7 +6628,7 @@
       <c r="T17"/>
       <c r="U17"/>
     </row>
-    <row r="18" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>207</v>
       </c>
@@ -6467,7 +6659,7 @@
       <c r="T18"/>
       <c r="U18"/>
     </row>
-    <row r="19" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>208</v>
       </c>
@@ -6495,31 +6687,31 @@
       <c r="T19"/>
       <c r="U19"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -6532,7 +6724,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -6545,7 +6737,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -6553,7 +6745,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -6561,7 +6753,7 @@
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -6569,7 +6761,7 @@
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -6590,18 +6782,18 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -6629,7 +6821,7 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>191</v>
       </c>
@@ -6646,7 +6838,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>192</v>
       </c>
@@ -6663,7 +6855,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>219</v>
       </c>
@@ -6683,7 +6875,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>201</v>
       </c>
@@ -6697,7 +6889,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>202</v>
       </c>
@@ -6711,7 +6903,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>227</v>
       </c>
@@ -6728,7 +6920,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>199</v>
       </c>
@@ -6742,7 +6934,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>209</v>
       </c>
@@ -6763,7 +6955,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>206</v>
       </c>
@@ -6784,7 +6976,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>210</v>
       </c>
@@ -6805,7 +6997,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>218</v>
       </c>
@@ -6826,7 +7018,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>223</v>
       </c>
@@ -6844,7 +7036,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -6858,7 +7050,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>207</v>
       </c>
@@ -6880,7 +7072,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>208</v>
       </c>
@@ -6889,7 +7081,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -6903,7 +7095,7 @@
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -6919,7 +7111,7 @@
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -6935,7 +7127,7 @@
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -6949,7 +7141,7 @@
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -6963,18 +7155,18 @@
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
     </row>
-    <row r="27" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="29" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="30" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added fire and ice explosion effects, Updated health Bar
Add fire and ice explosion effects for when they come in contact with an
enemy

Changed Experience algorithm

added sword to clerk

Updated magicIcon

Updated health bar to gradually bring health down

updated task list
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="337">
   <si>
     <t>Feature</t>
   </si>
@@ -981,12 +981,6 @@
     <t>When going in for an attack</t>
   </si>
   <si>
-    <t>Make things pop more ie particles</t>
-  </si>
-  <si>
-    <t>Improve visuals of attacking enemy, like health reducing make it wiggle/ show life</t>
-  </si>
-  <si>
     <t>Finished</t>
   </si>
   <si>
@@ -1030,6 +1024,30 @@
   </si>
   <si>
     <t>Have all icons rotate in the direction they are thrown</t>
+  </si>
+  <si>
+    <t>Fire trail and fire explosion</t>
+  </si>
+  <si>
+    <t>Add sound effect</t>
+  </si>
+  <si>
+    <t>Ice trail and explosion</t>
+  </si>
+  <si>
+    <t>Improve visuals of attacking enemy, like health reducing</t>
+  </si>
+  <si>
+    <t>Improve Inventory look</t>
+  </si>
+  <si>
+    <t>Make Video demonstrating game</t>
+  </si>
+  <si>
+    <t>Fix enemy pushing back when attacking and hit with ice</t>
+  </si>
+  <si>
+    <t>Fix Shield</t>
   </si>
 </sst>
 </file>
@@ -4874,10 +4892,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4930,10 +4948,10 @@
         <v>123</v>
       </c>
       <c r="G2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4953,10 +4971,10 @@
         <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4993,10 +5011,10 @@
         <v>123</v>
       </c>
       <c r="G5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5016,10 +5034,10 @@
         <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -5053,10 +5071,10 @@
         <v>123</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -5076,10 +5094,10 @@
         <v>123</v>
       </c>
       <c r="G9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -5099,31 +5117,46 @@
         <v>123</v>
       </c>
       <c r="G10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C13" s="14">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>123</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5131,148 +5164,119 @@
         <v>317</v>
       </c>
       <c r="C14" s="14">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>123</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C15" s="14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>123</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C16" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F16" s="28" t="s">
         <v>123</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C17" s="14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F17" s="28" t="s">
         <v>123</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="C18" s="14">
-        <v>2</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>316</v>
+        <v>328</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="F19" s="26" t="s">
+    </row>
+    <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="F22" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B21" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>14.5</v>
-      </c>
-      <c r="C21" s="14">
-        <f>SUM(C2:C20)</f>
-        <v>15.5</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B22" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>14.5</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="26" t="s">
+    <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="F24" s="26" t="s">
         <v>121</v>
       </c>
     </row>
@@ -5285,7 +5289,79 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="39" t="s">
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B26" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>14.5</v>
+      </c>
+      <c r="C26" s="14">
+        <f>SUM(C2:C25)</f>
+        <v>19.5</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>14.5</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="39" t="s">
         <v>279</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed CoinBag look, added lightning effect, fixed shield issue
New coin bag design

Added lightning effect (WIP)

Added fire explosion sound effect

Improved look of inventory, store, and start scene
Buttons indicate mode in inventory and store
Indicate equipped item in inventoryitemdetails

Fixed shield not being selectable

added a few more items to the clerk

Updated damagetext

Increased speed of rangedicon

Updated task list
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="336">
   <si>
     <t>Feature</t>
   </si>
@@ -951,9 +951,6 @@
     <t xml:space="preserve">Ice or fire not moving with enemy </t>
   </si>
   <si>
-    <t>Make more weapons and shields</t>
-  </si>
-  <si>
     <t>Improve colliders on enemies</t>
   </si>
   <si>
@@ -966,12 +963,6 @@
     <t>Fix damage done by damageovertime</t>
   </si>
   <si>
-    <t>Look into why Shield is so slow to be selected</t>
-  </si>
-  <si>
-    <t>Come up with new algorithm for experience</t>
-  </si>
-  <si>
     <t>Adjust enemy attack times, health, and speeds. Adjust Player stats, speed up icons, fix some issues affecting gameplay</t>
   </si>
   <si>
@@ -1023,15 +1014,9 @@
     <t>Added bow Graphic to rangedicons</t>
   </si>
   <si>
-    <t>Have all icons rotate in the direction they are thrown</t>
-  </si>
-  <si>
     <t>Fire trail and fire explosion</t>
   </si>
   <si>
-    <t>Add sound effect</t>
-  </si>
-  <si>
     <t>Ice trail and explosion</t>
   </si>
   <si>
@@ -1048,6 +1033,18 @@
   </si>
   <si>
     <t>Fix Shield</t>
+  </si>
+  <si>
+    <t>Icons disable when they can't be used</t>
+  </si>
+  <si>
+    <t>Improve Title screen</t>
+  </si>
+  <si>
+    <t>Redesigned coin bag</t>
+  </si>
+  <si>
+    <t>Create lightning effect</t>
   </si>
 </sst>
 </file>
@@ -4707,10 +4704,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4817,7 +4814,7 @@
         <v>309</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>106</v>
@@ -4825,63 +4822,21 @@
       <c r="F6" s="26" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>312</v>
-      </c>
-      <c r="B7">
-        <v>1.5</v>
+      <c r="G6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="14">
+        <v>10</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>304</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="B9" s="14">
-        <v>10</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>310</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="26" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4892,10 +4847,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4948,10 +4903,10 @@
         <v>123</v>
       </c>
       <c r="G2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4971,10 +4926,10 @@
         <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4991,7 +4946,7 @@
         <v>121</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5011,10 +4966,10 @@
         <v>123</v>
       </c>
       <c r="G5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5034,10 +4989,10 @@
         <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -5056,7 +5011,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -5071,15 +5026,15 @@
         <v>123</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -5094,15 +5049,15 @@
         <v>123</v>
       </c>
       <c r="G9" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H9" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B10">
         <v>2.5</v>
@@ -5117,12 +5072,12 @@
         <v>123</v>
       </c>
       <c r="G10" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5133,7 +5088,7 @@
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C12" s="14">
         <v>1.5</v>
@@ -5142,12 +5097,12 @@
         <v>123</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C13" s="14">
         <v>5</v>
@@ -5156,12 +5111,12 @@
         <v>123</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C14" s="14">
         <v>0.5</v>
@@ -5170,12 +5125,12 @@
         <v>123</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C15" s="14">
         <v>1</v>
@@ -5184,12 +5139,12 @@
         <v>123</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C16" s="14">
         <v>0.5</v>
@@ -5198,12 +5153,12 @@
         <v>123</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C17" s="14">
         <v>2</v>
@@ -5212,37 +5167,37 @@
         <v>123</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>121</v>
+        <v>325</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C19" s="14">
         <v>1.5</v>
       </c>
-      <c r="F19" s="39" t="s">
-        <v>279</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>330</v>
+      <c r="F19" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C20" s="14">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F20" s="28" t="s">
         <v>123</v>
@@ -5250,15 +5205,18 @@
     </row>
     <row r="21" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="F21" s="39" t="s">
-        <v>279</v>
+        <v>329</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>334</v>
+        <v>330</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1.5</v>
       </c>
       <c r="F22" s="26" t="s">
         <v>121</v>
@@ -5266,77 +5224,65 @@
     </row>
     <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>121</v>
+        <v>331</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F24" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B26" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>14.5</v>
+        <v>334</v>
       </c>
       <c r="C26" s="14">
-        <f>SUM(C2:C25)</f>
-        <v>19.5</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B27" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>14.5</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="28" t="s">
-        <v>123</v>
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="C27" s="14">
+        <v>2</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -5348,20 +5294,79 @@
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
-      <c r="I29" s="26" t="s">
-        <v>121</v>
-      </c>
+      <c r="I29" s="14"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="A30" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>14.5</v>
+      </c>
+      <c r="C30" s="14">
+        <f>SUM(C2:C29)</f>
+        <v>30</v>
+      </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
-      <c r="I30" s="39" t="s">
+      <c r="I30" s="14"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B31" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>14.5</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="39" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5521,7 +5526,7 @@
         <v>279</v>
       </c>
       <c r="G7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Loading Screen, icons disable when they cannot be used
Added Loading Screen

Icons disable when they cannot be used, same with controls

New icons spawn in when the slot is out of view of the camera

Lightning bolt follows the enemy

Added arrow trajectory renderer to render arrows path

Updated task list
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="339">
   <si>
     <t>Feature</t>
   </si>
@@ -1045,6 +1045,15 @@
   </si>
   <si>
     <t>Create lightning effect</t>
+  </si>
+  <si>
+    <t>Draw trajectory path for arrows</t>
+  </si>
+  <si>
+    <t>Add Loading screen</t>
+  </si>
+  <si>
+    <t>New icons spawn in when slot is out of camera</t>
   </si>
 </sst>
 </file>
@@ -4511,7 +4520,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4547,7 +4556,7 @@
         <v>297</v>
       </c>
       <c r="C2" s="36">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -4582,11 +4591,11 @@
       <c r="B5" t="s">
         <v>264</v>
       </c>
-      <c r="C5" s="36">
-        <v>0.9</v>
+      <c r="C5" s="36" t="s">
+        <v>275</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4596,11 +4605,11 @@
       <c r="B6" t="s">
         <v>264</v>
       </c>
-      <c r="C6" s="36">
-        <v>0.9</v>
+      <c r="C6" s="36" t="s">
+        <v>275</v>
       </c>
       <c r="D6" s="14">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4847,10 +4856,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5082,6 +5091,9 @@
       <c r="C11">
         <v>1</v>
       </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F11" s="28" t="s">
         <v>123</v>
       </c>
@@ -5093,6 +5105,9 @@
       <c r="C12" s="14">
         <v>1.5</v>
       </c>
+      <c r="E12" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F12" s="28" t="s">
         <v>123</v>
       </c>
@@ -5107,6 +5122,9 @@
       <c r="C13" s="14">
         <v>5</v>
       </c>
+      <c r="E13" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F13" s="28" t="s">
         <v>123</v>
       </c>
@@ -5121,6 +5139,9 @@
       <c r="C14" s="14">
         <v>0.5</v>
       </c>
+      <c r="E14" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F14" s="28" t="s">
         <v>123</v>
       </c>
@@ -5135,6 +5156,9 @@
       <c r="C15" s="14">
         <v>1</v>
       </c>
+      <c r="E15" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F15" s="28" t="s">
         <v>123</v>
       </c>
@@ -5149,6 +5173,9 @@
       <c r="C16" s="14">
         <v>0.5</v>
       </c>
+      <c r="E16" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F16" s="28" t="s">
         <v>123</v>
       </c>
@@ -5163,6 +5190,9 @@
       <c r="C17" s="14">
         <v>2</v>
       </c>
+      <c r="E17" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F17" s="28" t="s">
         <v>123</v>
       </c>
@@ -5177,6 +5207,9 @@
       <c r="C18" s="14">
         <v>2</v>
       </c>
+      <c r="E18" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F18" s="28" t="s">
         <v>123</v>
       </c>
@@ -5188,6 +5221,9 @@
       <c r="C19" s="14">
         <v>1.5</v>
       </c>
+      <c r="E19" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F19" s="28" t="s">
         <v>123</v>
       </c>
@@ -5199,6 +5235,9 @@
       <c r="C20" s="14">
         <v>3</v>
       </c>
+      <c r="E20" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F20" s="28" t="s">
         <v>123</v>
       </c>
@@ -5207,6 +5246,9 @@
       <c r="A21" s="14" t="s">
         <v>329</v>
       </c>
+      <c r="E21" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F21" s="26" t="s">
         <v>121</v>
       </c>
@@ -5218,6 +5260,9 @@
       <c r="C22" s="14">
         <v>1.5</v>
       </c>
+      <c r="E22" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F22" s="26" t="s">
         <v>121</v>
       </c>
@@ -5229,6 +5274,9 @@
       <c r="C23" s="14">
         <v>1</v>
       </c>
+      <c r="E23" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F23" s="28" t="s">
         <v>123</v>
       </c>
@@ -5237,8 +5285,14 @@
       <c r="A24" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="F24" s="26" t="s">
-        <v>121</v>
+      <c r="C24" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5248,6 +5302,9 @@
       <c r="C25" s="14">
         <v>1</v>
       </c>
+      <c r="E25" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F25" s="28" t="s">
         <v>123</v>
       </c>
@@ -5259,6 +5316,9 @@
       <c r="C26" s="14">
         <v>0.5</v>
       </c>
+      <c r="E26" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F26" s="28" t="s">
         <v>123</v>
       </c>
@@ -5268,10 +5328,16 @@
         <v>335</v>
       </c>
       <c r="C27" s="14">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="F27" s="28" t="s">
         <v>123</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5279,57 +5345,53 @@
         <v>298</v>
       </c>
       <c r="C28" s="14">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="F28" s="39" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B30" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>14.5</v>
+        <v>337</v>
       </c>
       <c r="C30" s="14">
-        <f>SUM(C2:C29)</f>
-        <v>30</v>
-      </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B31" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>14.5</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="C31" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
@@ -5340,33 +5402,79 @@
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
-      <c r="I32" s="28" t="s">
-        <v>123</v>
-      </c>
+      <c r="I32" s="14"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="A33" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>14.5</v>
+      </c>
+      <c r="C33" s="14">
+        <f>SUM(C2:C32)</f>
+        <v>37</v>
+      </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
-      <c r="I33" s="26" t="s">
-        <v>121</v>
-      </c>
+      <c r="I33" s="14"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B34" s="14">
+        <f>SUM(B2:B11)</f>
+        <v>14.5</v>
+      </c>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
-      <c r="I34" s="39" t="s">
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="39" t="s">
         <v>279</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Sound Effects to Player, updated itemdatabase
Added sound effects to Player

Updated itemdatabase

Updated some enemy prefabs

Reduced the size of collider on SteelSword

Added loading screen to all scenes

Changed algorithm for enemy attack movement to work better with slow
down effect of ice

Prevent controls from being used after level is over

Changed repair hammer to repair shield fully

Updated Task List
</commit_message>
<xml_diff>
--- a/TechnicalDesign/Task List For RPG Hero.xlsx
+++ b/TechnicalDesign/Task List For RPG Hero.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="339">
   <si>
     <t>Feature</t>
   </si>
@@ -939,9 +939,6 @@
     <t>Push Perspective back/Add Layers to enemy positions</t>
   </si>
   <si>
-    <t>Add visual indications that the player has been hit</t>
-  </si>
-  <si>
     <t>Unlock levels as you progress</t>
   </si>
   <si>
@@ -957,9 +954,6 @@
     <t>Add back button to scenes</t>
   </si>
   <si>
-    <t>Blocking with shield, player being hit, player dies, etc</t>
-  </si>
-  <si>
     <t>Fix damage done by damageovertime</t>
   </si>
   <si>
@@ -1020,9 +1014,6 @@
     <t>Ice trail and explosion</t>
   </si>
   <si>
-    <t>Improve visuals of attacking enemy, like health reducing</t>
-  </si>
-  <si>
     <t>Improve Inventory look</t>
   </si>
   <si>
@@ -1054,6 +1045,15 @@
   </si>
   <si>
     <t>New icons spawn in when slot is out of camera</t>
+  </si>
+  <si>
+    <t>Blocking with shield, player being hit, Player wins and player dies</t>
+  </si>
+  <si>
+    <t>Health bar reduce gradual</t>
+  </si>
+  <si>
+    <t>Disable icons after level ends</t>
   </si>
 </sst>
 </file>
@@ -4820,7 +4820,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B6">
         <v>1.5</v>
@@ -4832,7 +4832,7 @@
         <v>121</v>
       </c>
       <c r="G6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4858,8 +4858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4912,10 +4912,10 @@
         <v>123</v>
       </c>
       <c r="G2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4935,10 +4935,10 @@
         <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4948,19 +4948,22 @@
       <c r="B4" s="14">
         <v>2</v>
       </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>121</v>
+      <c r="F4" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>306</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4975,15 +4978,15 @@
         <v>123</v>
       </c>
       <c r="G5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4998,35 +5001,44 @@
         <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
         <v>1</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>121</v>
+      <c r="F7" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="H7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>106</v>
@@ -5034,22 +5046,22 @@
       <c r="F8" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="14" t="s">
-        <v>311</v>
+      <c r="G8" t="s">
+        <v>309</v>
       </c>
       <c r="H8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>106</v>
@@ -5058,52 +5070,46 @@
         <v>123</v>
       </c>
       <c r="G9" t="s">
-        <v>311</v>
-      </c>
-      <c r="H9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>305</v>
-      </c>
-      <c r="B10">
-        <v>2.5</v>
+        <v>337</v>
       </c>
       <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C11" s="14">
         <v>1.5</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>327</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
       <c r="E11" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F11" s="28" t="s">
         <v>123</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C12" s="14">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>106</v>
@@ -5112,7 +5118,7 @@
         <v>123</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5120,7 +5126,7 @@
         <v>312</v>
       </c>
       <c r="C13" s="14">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>106</v>
@@ -5129,15 +5135,15 @@
         <v>123</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="C14" s="14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>106</v>
@@ -5146,15 +5152,15 @@
         <v>123</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C15" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>106</v>
@@ -5163,15 +5169,15 @@
         <v>123</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C16" s="14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>106</v>
@@ -5180,12 +5186,12 @@
         <v>123</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C17" s="14">
         <v>2</v>
@@ -5195,17 +5201,14 @@
       </c>
       <c r="F17" s="28" t="s">
         <v>123</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C18" s="14">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>106</v>
@@ -5216,10 +5219,10 @@
     </row>
     <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C19" s="14">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>106</v>
@@ -5230,10 +5233,10 @@
     </row>
     <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C20" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>106</v>
@@ -5244,35 +5247,38 @@
     </row>
     <row r="21" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
+      </c>
+      <c r="C21" s="14">
+        <v>3</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="26" t="s">
-        <v>121</v>
+      <c r="F21" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C22" s="14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F22" s="26" t="s">
-        <v>121</v>
+      <c r="F22" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C23" s="14">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>106</v>
@@ -5283,10 +5289,10 @@
     </row>
     <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C24" s="14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>106</v>
@@ -5297,10 +5303,10 @@
     </row>
     <row r="25" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C25" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>106</v>
@@ -5311,52 +5317,52 @@
     </row>
     <row r="26" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C26" s="14">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="28" t="s">
         <v>123</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
       <c r="C27" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F27" s="28" t="s">
         <v>123</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>298</v>
+        <v>333</v>
       </c>
       <c r="C28" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F28" s="39" t="s">
-        <v>279</v>
+      <c r="F28" s="28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C29" s="14">
         <v>1</v>
@@ -5370,10 +5376,10 @@
     </row>
     <row r="30" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C30" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>106</v>
@@ -5388,6 +5394,9 @@
       </c>
       <c r="C31" s="14">
         <v>0.5</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="F31" s="28" t="s">
         <v>123</v>
@@ -5409,12 +5418,12 @@
         <v>207</v>
       </c>
       <c r="B33" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>14.5</v>
+        <f>SUM(B2:B10)</f>
+        <v>13.5</v>
       </c>
       <c r="C33" s="14">
         <f>SUM(C2:C32)</f>
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
@@ -5428,8 +5437,8 @@
         <v>208</v>
       </c>
       <c r="B34" s="14">
-        <f>SUM(B2:B11)</f>
-        <v>14.5</v>
+        <f>SUM(B2:B10)</f>
+        <v>13.5</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
@@ -5634,7 +5643,7 @@
         <v>279</v>
       </c>
       <c r="G7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -5659,7 +5668,7 @@
     </row>
     <row r="9" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B9" s="38">
         <v>1</v>

</xml_diff>